<commit_message>
Fix items bug showing duplicates
</commit_message>
<xml_diff>
--- a/database/7052/JobSummary.xlsx
+++ b/database/7052/JobSummary.xlsx
@@ -4432,21 +4432,21 @@
       <c r="B1" s="61" t="n"/>
       <c r="C1" s="58" t="inlineStr">
         <is>
-          <t>981 Spools</t>
+          <t>1019 Spools</t>
         </is>
       </c>
       <c r="D1" s="61" t="n"/>
       <c r="E1" s="49" t="n"/>
       <c r="F1" s="58" t="inlineStr">
         <is>
-          <t>30 Workable</t>
+          <t>185 Workable</t>
         </is>
       </c>
       <c r="G1" s="61" t="n"/>
       <c r="H1" s="49" t="n"/>
       <c r="I1" s="58" t="inlineStr">
         <is>
-          <t>30 Issued</t>
+          <t>187 Issued</t>
         </is>
       </c>
       <c r="J1" s="61" t="n"/>
@@ -5462,10 +5462,10 @@
         <v>0</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>0</v>
@@ -5484,7 +5484,7 @@
       </c>
       <c r="L33" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="M33" s="1" t="inlineStr">
@@ -5510,22 +5510,22 @@
         </is>
       </c>
       <c r="C34" s="1" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>0</v>
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
@@ -5570,10 +5570,10 @@
         <v>5</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>0</v>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>71.1%</t>
         </is>
       </c>
       <c r="M35" s="1" t="inlineStr">
@@ -5621,19 +5621,19 @@
         <v>242</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>0</v>
@@ -5646,12 +5646,12 @@
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>23.6%</t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="N36" s="1" t="inlineStr">
@@ -5672,22 +5672,22 @@
         </is>
       </c>
       <c r="C37" s="1" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>0</v>
@@ -5696,11 +5696,11 @@
         <v>0</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L37" s="1" t="inlineStr">
         <is>
-          <t>6.2%</t>
+          <t>24.1%</t>
         </is>
       </c>
       <c r="M37" s="1" t="inlineStr">
@@ -5726,22 +5726,22 @@
         </is>
       </c>
       <c r="C38" s="1" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>0</v>
@@ -5750,11 +5750,11 @@
         <v>0</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L38" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>16.0%</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
@@ -5783,19 +5783,19 @@
         <v>42</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E39" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="G39" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="H39" s="1" t="n">
         <v>40</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>42</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>0</v>
@@ -5808,12 +5808,12 @@
       </c>
       <c r="L39" s="1" t="inlineStr">
         <is>
+          <t>35.7%</t>
+        </is>
+      </c>
+      <c r="M39" s="1" t="inlineStr">
+        <is>
           <t>4.8%</t>
-        </is>
-      </c>
-      <c r="M39" s="1" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N39" s="1" t="inlineStr">
@@ -5837,13 +5837,13 @@
         <v>21</v>
       </c>
       <c r="D40" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E40" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="F40" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>0</v>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="L40" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9.5%</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
@@ -5888,22 +5888,22 @@
         </is>
       </c>
       <c r="C41" s="1" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="G41" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F41" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="G41" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="H41" s="1" t="n">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>0</v>
@@ -5912,16 +5912,16 @@
         <v>0</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L41" s="1" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>8.3%</t>
         </is>
       </c>
       <c r="M41" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.4%</t>
         </is>
       </c>
       <c r="N41" s="1" t="inlineStr">
@@ -5954,10 +5954,10 @@
         <v>41</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>0</v>
@@ -5975,7 +5975,7 @@
       </c>
       <c r="M42" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>2.4%</t>
         </is>
       </c>
       <c r="N42" s="1" t="inlineStr">
@@ -6053,13 +6053,13 @@
         <v>10</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>0</v>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="L44" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10.0%</t>
         </is>
       </c>
       <c r="M44" s="1" t="inlineStr">
@@ -6164,10 +6164,10 @@
         <v>0</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1" t="n">
         <v>0</v>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="L46" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>11.1%</t>
         </is>
       </c>
       <c r="M46" s="1" t="inlineStr">
@@ -6212,22 +6212,22 @@
         </is>
       </c>
       <c r="C47" s="1" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E47" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="G47" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F47" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="H47" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I47" s="1" t="n">
         <v>0</v>
@@ -6236,16 +6236,16 @@
         <v>0</v>
       </c>
       <c r="K47" s="1" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L47" s="1" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>22.7%</t>
         </is>
       </c>
       <c r="M47" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>9.1%</t>
         </is>
       </c>
       <c r="N47" s="1" t="inlineStr">
@@ -6266,19 +6266,19 @@
         </is>
       </c>
       <c r="C48" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E48" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G48" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="F48" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="G48" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="H48" s="1" t="n">
         <v>23</v>
@@ -6290,16 +6290,16 @@
         <v>0</v>
       </c>
       <c r="K48" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L48" s="1" t="inlineStr">
         <is>
-          <t>8.7%</t>
+          <t>44.0%</t>
         </is>
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>8.0%</t>
         </is>
       </c>
       <c r="N48" s="1" t="inlineStr">
@@ -6320,19 +6320,19 @@
         </is>
       </c>
       <c r="C49" s="1" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H49" s="1" t="n">
         <v>49</v>
@@ -6344,16 +6344,16 @@
         <v>0</v>
       </c>
       <c r="K49" s="1" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L49" s="1" t="inlineStr">
         <is>
-          <t>4.1%</t>
+          <t>17.0%</t>
         </is>
       </c>
       <c r="M49" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>7.5%</t>
         </is>
       </c>
       <c r="N49" s="1" t="inlineStr">
@@ -6422,22 +6422,22 @@
       </c>
       <c r="B51" s="64" t="n"/>
       <c r="C51" s="64" t="n">
-        <v>981</v>
+        <v>1019</v>
       </c>
       <c r="D51" s="64" t="n">
-        <v>370</v>
+        <v>292</v>
       </c>
       <c r="E51" s="64" t="n">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="F51" s="64" t="n">
-        <v>951</v>
+        <v>834</v>
       </c>
       <c r="G51" s="64" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H51" s="64" t="n">
-        <v>981</v>
+        <v>995</v>
       </c>
       <c r="I51" s="64" t="n">
         <v>0</v>
@@ -6446,16 +6446,16 @@
         <v>0</v>
       </c>
       <c r="K51" s="64" t="n">
-        <v>981</v>
+        <v>1019</v>
       </c>
       <c r="L51" s="64" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="M51" s="64" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="N51" s="64" t="inlineStr">
@@ -6489,7 +6489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -6523,6 +6523,96 @@
           <t>PM In Status Report (Not in Line List)</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>44-2</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>48-1</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>52-2</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>341-1</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>401-1</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>401-2</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>401-3</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>401-4</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>463-4</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6657,10 +6747,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
@@ -6679,7 +6769,7 @@
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
@@ -6705,22 +6795,22 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>0</v>
@@ -6729,7 +6819,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
@@ -6765,10 +6855,10 @@
         <v>5</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>0</v>
@@ -6787,7 +6877,7 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>71.1%</t>
         </is>
       </c>
       <c r="M5" s="5" t="inlineStr">
@@ -6816,19 +6906,19 @@
         <v>242</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -6841,12 +6931,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>23.6%</t>
         </is>
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -6867,22 +6957,22 @@
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I7" s="5" t="n">
         <v>0</v>
@@ -6891,11 +6981,11 @@
         <v>0</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>6.2%</t>
+          <t>24.1%</t>
         </is>
       </c>
       <c r="M7" s="5" t="inlineStr">
@@ -6921,22 +7011,22 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I8" s="5" t="n">
         <v>0</v>
@@ -6945,11 +7035,11 @@
         <v>0</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>16.0%</t>
         </is>
       </c>
       <c r="M8" s="5" t="inlineStr">
@@ -6978,19 +7068,19 @@
         <v>42</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="G9" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="H9" s="5" t="n">
         <v>40</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>42</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>0</v>
@@ -7003,12 +7093,12 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
+          <t>35.7%</t>
+        </is>
+      </c>
+      <c r="M9" s="5" t="inlineStr">
+        <is>
           <t>4.8%</t>
-        </is>
-      </c>
-      <c r="M9" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N9" s="5" t="inlineStr">
@@ -7032,13 +7122,13 @@
         <v>21</v>
       </c>
       <c r="D10" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="F10" s="5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
@@ -7057,7 +7147,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9.5%</t>
         </is>
       </c>
       <c r="M10" s="5" t="inlineStr">
@@ -7083,22 +7173,22 @@
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E11" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>143</v>
+      </c>
+      <c r="G11" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="n">
-        <v>144</v>
-      </c>
-      <c r="G11" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="H11" s="5" t="n">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I11" s="5" t="n">
         <v>0</v>
@@ -7107,16 +7197,16 @@
         <v>0</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L11" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>8.3%</t>
         </is>
       </c>
       <c r="M11" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.4%</t>
         </is>
       </c>
       <c r="N11" s="5" t="inlineStr">
@@ -7149,10 +7239,10 @@
         <v>41</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
@@ -7170,7 +7260,7 @@
       </c>
       <c r="M12" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>2.4%</t>
         </is>
       </c>
       <c r="N12" s="5" t="inlineStr">
@@ -7248,13 +7338,13 @@
         <v>10</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
@@ -7273,7 +7363,7 @@
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10.0%</t>
         </is>
       </c>
       <c r="M14" s="5" t="inlineStr">
@@ -7359,10 +7449,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
@@ -7381,7 +7471,7 @@
       </c>
       <c r="L16" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>11.1%</t>
         </is>
       </c>
       <c r="M16" s="5" t="inlineStr">
@@ -7407,22 +7497,22 @@
         </is>
       </c>
       <c r="C17" s="5" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="G17" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="G17" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="H17" s="5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -7431,16 +7521,16 @@
         <v>0</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>22.7%</t>
         </is>
       </c>
       <c r="M17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>9.1%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -7461,19 +7551,19 @@
         </is>
       </c>
       <c r="C18" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5" t="n">
         <v>2</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="G18" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="H18" s="5" t="n">
         <v>23</v>
@@ -7485,16 +7575,16 @@
         <v>0</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
-          <t>8.7%</t>
+          <t>44.0%</t>
         </is>
       </c>
       <c r="M18" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>8.0%</t>
         </is>
       </c>
       <c r="N18" s="5" t="inlineStr">
@@ -7515,19 +7605,19 @@
         </is>
       </c>
       <c r="C19" s="5" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H19" s="5" t="n">
         <v>49</v>
@@ -7539,16 +7629,16 @@
         <v>0</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>4.1%</t>
+          <t>17.0%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>7.5%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -7617,22 +7707,22 @@
       </c>
       <c r="B21" s="67" t="n"/>
       <c r="C21" s="67" t="n">
-        <v>981</v>
+        <v>1019</v>
       </c>
       <c r="D21" s="67" t="n">
-        <v>370</v>
+        <v>292</v>
       </c>
       <c r="E21" s="67" t="n">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="F21" s="67" t="n">
-        <v>951</v>
+        <v>834</v>
       </c>
       <c r="G21" s="67" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H21" s="67" t="n">
-        <v>981</v>
+        <v>995</v>
       </c>
       <c r="I21" s="67" t="n">
         <v>0</v>
@@ -7641,16 +7731,16 @@
         <v>0</v>
       </c>
       <c r="K21" s="67" t="n">
-        <v>981</v>
+        <v>1019</v>
       </c>
       <c r="L21" s="67" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="M21" s="67" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="N21" s="67" t="inlineStr">
@@ -7673,7 +7763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
@@ -7788,22 +7878,22 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E3" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>139</v>
+      </c>
+      <c r="G3" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <v>140</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="H3" s="5" t="n">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>0</v>
@@ -7812,16 +7902,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>6.7%</t>
+          <t>8.6%</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.6%</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
@@ -7854,10 +7944,10 @@
         <v>41</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>0</v>
@@ -7875,7 +7965,7 @@
       </c>
       <c r="M4" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>2.4%</t>
         </is>
       </c>
       <c r="N4" s="5" t="inlineStr">
@@ -7902,16 +7992,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="H5" s="5" t="n">
         <v>11</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>13</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
@@ -7924,12 +8014,12 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
+          <t>30.8%</t>
+        </is>
+      </c>
+      <c r="M5" s="5" t="inlineStr">
+        <is>
           <t>15.4%</t>
-        </is>
-      </c>
-      <c r="M5" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
@@ -7953,19 +8043,19 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E6" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="H6" s="5" t="n">
         <v>10</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>12</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -7978,12 +8068,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
+          <t>25.0%</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
           <t>16.7%</t>
-        </is>
-      </c>
-      <c r="M6" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -8007,13 +8097,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
@@ -8032,7 +8122,7 @@
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10.5%</t>
         </is>
       </c>
       <c r="M7" s="5" t="inlineStr">
@@ -8054,22 +8144,22 @@
       </c>
       <c r="B8" s="67" t="n"/>
       <c r="C8" s="67" t="n">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D8" s="67" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E8" s="67" t="n">
+        <v>25</v>
+      </c>
+      <c r="F8" s="67" t="n">
+        <v>232</v>
+      </c>
+      <c r="G8" s="67" t="n">
         <v>15</v>
       </c>
-      <c r="F8" s="67" t="n">
-        <v>240</v>
-      </c>
-      <c r="G8" s="67" t="n">
-        <v>0</v>
-      </c>
       <c r="H8" s="67" t="n">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="I8" s="67" t="n">
         <v>0</v>
@@ -8078,16 +8168,16 @@
         <v>0</v>
       </c>
       <c r="K8" s="67" t="n">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L8" s="67" t="inlineStr">
         <is>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="M8" s="67" t="inlineStr">
+        <is>
           <t>6%</t>
-        </is>
-      </c>
-      <c r="M8" s="67" t="inlineStr">
-        <is>
-          <t>0%</t>
         </is>
       </c>
       <c r="N8" s="67" t="inlineStr">
@@ -8203,22 +8293,22 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
@@ -8227,11 +8317,11 @@
         <v>0</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>20.0%</t>
         </is>
       </c>
       <c r="M12" s="5" t="inlineStr">
@@ -8257,22 +8347,22 @@
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I13" s="5" t="n">
         <v>0</v>
@@ -8281,11 +8371,11 @@
         <v>0</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L13" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>58.3%</t>
         </is>
       </c>
       <c r="M13" s="5" t="inlineStr">
@@ -8317,16 +8407,16 @@
         <v>0</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>0</v>
@@ -8339,12 +8429,12 @@
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>25.0%</t>
         </is>
       </c>
       <c r="M14" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>7.1%</t>
         </is>
       </c>
       <c r="N14" s="5" t="inlineStr">
@@ -8371,10 +8461,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>0</v>
@@ -8393,7 +8483,7 @@
       </c>
       <c r="L15" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="M15" s="5" t="inlineStr">
@@ -8425,10 +8515,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
@@ -8447,7 +8537,7 @@
       </c>
       <c r="L16" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>11.1%</t>
         </is>
       </c>
       <c r="M16" s="5" t="inlineStr">
@@ -8479,10 +8569,10 @@
         <v>5</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>0</v>
@@ -8501,7 +8591,7 @@
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>71.1%</t>
         </is>
       </c>
       <c r="M17" s="5" t="inlineStr">
@@ -8582,19 +8672,19 @@
         <v>204</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>198</v>
+        <v>151</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I19" s="5" t="n">
         <v>0</v>
@@ -8607,12 +8697,12 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>2.9%</t>
+          <t>26.0%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>1.5%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -8633,22 +8723,22 @@
         </is>
       </c>
       <c r="C20" s="5" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I20" s="5" t="n">
         <v>0</v>
@@ -8657,11 +8747,11 @@
         <v>0</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L20" s="5" t="inlineStr">
         <is>
-          <t>7.0%</t>
+          <t>27.4%</t>
         </is>
       </c>
       <c r="M20" s="5" t="inlineStr">
@@ -8687,22 +8777,22 @@
         </is>
       </c>
       <c r="C21" s="5" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I21" s="5" t="n">
         <v>0</v>
@@ -8711,11 +8801,11 @@
         <v>0</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L21" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>22.7%</t>
         </is>
       </c>
       <c r="M21" s="5" t="inlineStr">
@@ -8747,16 +8837,16 @@
         <v>0</v>
       </c>
       <c r="E22" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G22" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="H22" s="5" t="n">
         <v>18</v>
-      </c>
-      <c r="G22" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5" t="n">
-        <v>20</v>
       </c>
       <c r="I22" s="5" t="n">
         <v>0</v>
@@ -8769,12 +8859,12 @@
       </c>
       <c r="L22" s="5" t="inlineStr">
         <is>
+          <t>70.0%</t>
+        </is>
+      </c>
+      <c r="M22" s="5" t="inlineStr">
+        <is>
           <t>10.0%</t>
-        </is>
-      </c>
-      <c r="M22" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N22" s="5" t="inlineStr">
@@ -8798,13 +8888,13 @@
         <v>11</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>0</v>
@@ -8823,7 +8913,7 @@
       </c>
       <c r="L23" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>9.1%</t>
         </is>
       </c>
       <c r="M23" s="5" t="inlineStr">
@@ -8906,13 +8996,13 @@
         <v>10</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25" s="5" t="n">
         <v>0</v>
@@ -8931,7 +9021,7 @@
       </c>
       <c r="L25" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10.0%</t>
         </is>
       </c>
       <c r="M25" s="5" t="inlineStr">
@@ -9007,22 +9097,22 @@
       </c>
       <c r="B27" s="67" t="n"/>
       <c r="C27" s="67" t="n">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="D27" s="67" t="n">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="E27" s="67" t="n">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="F27" s="67" t="n">
-        <v>483</v>
+        <v>350</v>
       </c>
       <c r="G27" s="67" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H27" s="67" t="n">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="I27" s="67" t="n">
         <v>0</v>
@@ -9031,16 +9121,16 @@
         <v>0</v>
       </c>
       <c r="K27" s="67" t="n">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="L27" s="67" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>31%</t>
         </is>
       </c>
       <c r="M27" s="67" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="N27" s="67" t="inlineStr">
@@ -9168,10 +9258,10 @@
         <v>2</v>
       </c>
       <c r="G31" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I31" s="5" t="n">
         <v>0</v>
@@ -9189,7 +9279,7 @@
       </c>
       <c r="M31" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="N31" s="5" t="inlineStr">
@@ -9216,10 +9306,10 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" s="5" t="n">
         <v>0</v>
@@ -9238,7 +9328,7 @@
       </c>
       <c r="L32" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>10.0%</t>
         </is>
       </c>
       <c r="M32" s="5" t="inlineStr">
@@ -9270,10 +9360,10 @@
         <v>7</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33" s="5" t="n">
         <v>0</v>
@@ -9292,7 +9382,7 @@
       </c>
       <c r="L33" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>8.3%</t>
         </is>
       </c>
       <c r="M33" s="5" t="inlineStr">
@@ -9320,16 +9410,16 @@
         <v>7</v>
       </c>
       <c r="E34" s="67" t="n">
+        <v>4</v>
+      </c>
+      <c r="F34" s="67" t="n">
+        <v>22</v>
+      </c>
+      <c r="G34" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F34" s="67" t="n">
+      <c r="H34" s="67" t="n">
         <v>24</v>
-      </c>
-      <c r="G34" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="67" t="n">
-        <v>26</v>
       </c>
       <c r="I34" s="67" t="n">
         <v>0</v>
@@ -9342,12 +9432,12 @@
       </c>
       <c r="L34" s="67" t="inlineStr">
         <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="M34" s="67" t="inlineStr">
+        <is>
           <t>8%</t>
-        </is>
-      </c>
-      <c r="M34" s="67" t="inlineStr">
-        <is>
-          <t>0%</t>
         </is>
       </c>
       <c r="N34" s="67" t="inlineStr">
@@ -9463,22 +9553,22 @@
         </is>
       </c>
       <c r="C38" s="5" t="n">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="D38" s="5" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="5" t="n">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="G38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="5" t="n">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="I38" s="5" t="n">
         <v>0</v>
@@ -9487,7 +9577,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="5" t="n">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="L38" s="5" t="inlineStr">
         <is>
@@ -9517,7 +9607,7 @@
         </is>
       </c>
       <c r="C39" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>0</v>
@@ -9526,13 +9616,13 @@
         <v>0</v>
       </c>
       <c r="F39" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I39" s="5" t="n">
         <v>0</v>
@@ -9541,7 +9631,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L39" s="5" t="inlineStr">
         <is>
@@ -9675,22 +9765,22 @@
       </c>
       <c r="B42" s="67" t="n"/>
       <c r="C42" s="67" t="n">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="D42" s="67" t="n">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="E42" s="67" t="n">
         <v>0</v>
       </c>
       <c r="F42" s="67" t="n">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="G42" s="67" t="n">
         <v>0</v>
       </c>
       <c r="H42" s="67" t="n">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="I42" s="67" t="n">
         <v>0</v>
@@ -9699,7 +9789,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="67" t="n">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="L42" s="67" t="inlineStr">
         <is>
@@ -9881,7 +9971,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>0</v>
@@ -9931,7 +10021,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="67" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E48" s="67" t="n">
         <v>0</v>
@@ -10223,14 +10313,214 @@
         </is>
       </c>
     </row>
+    <row r="55" ht="15" customHeight="1">
+      <c r="A55" s="5" t="n"/>
+      <c r="B55" s="5" t="n"/>
+      <c r="C55" s="5" t="n"/>
+      <c r="D55" s="5" t="n"/>
+      <c r="E55" s="5" t="n"/>
+      <c r="F55" s="5" t="n"/>
+      <c r="G55" s="5" t="n"/>
+      <c r="H55" s="5" t="n"/>
+      <c r="I55" s="5" t="n"/>
+      <c r="J55" s="5" t="n"/>
+      <c r="K55" s="5" t="n"/>
+      <c r="L55" s="5" t="n"/>
+      <c r="M55" s="5" t="n"/>
+      <c r="N55" s="5" t="n"/>
+    </row>
+    <row r="56" ht="37" customHeight="1">
+      <c r="A56" s="65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="37" customHeight="1">
+      <c r="A57" s="66" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="B57" s="66" t="inlineStr">
+        <is>
+          <t>Priority #</t>
+        </is>
+      </c>
+      <c r="C57" s="66" t="inlineStr">
+        <is>
+          <t>Total Spools</t>
+        </is>
+      </c>
+      <c r="D57" s="66" t="inlineStr">
+        <is>
+          <t>On Hold</t>
+        </is>
+      </c>
+      <c r="E57" s="66" t="inlineStr">
+        <is>
+          <t>Workable</t>
+        </is>
+      </c>
+      <c r="F57" s="66" t="inlineStr">
+        <is>
+          <t>Not Workable</t>
+        </is>
+      </c>
+      <c r="G57" s="66" t="inlineStr">
+        <is>
+          <t>Welded Out</t>
+        </is>
+      </c>
+      <c r="H57" s="66" t="inlineStr">
+        <is>
+          <t>Remaining to Weld Out</t>
+        </is>
+      </c>
+      <c r="I57" s="66" t="inlineStr">
+        <is>
+          <t>Shipped To Paint</t>
+        </is>
+      </c>
+      <c r="J57" s="66" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="K57" s="66" t="inlineStr">
+        <is>
+          <t>Remaining to Deliver</t>
+        </is>
+      </c>
+      <c r="L57" s="66" t="inlineStr">
+        <is>
+          <t>Workable %</t>
+        </is>
+      </c>
+      <c r="M57" s="66" t="inlineStr">
+        <is>
+          <t>Weld Out %</t>
+        </is>
+      </c>
+      <c r="N57" s="66" t="inlineStr">
+        <is>
+          <t>Delivered %</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="15" customHeight="1">
+      <c r="A58" s="5" t="inlineStr">
+        <is>
+          <t>J14</t>
+        </is>
+      </c>
+      <c r="B58" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C58" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" s="5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="M58" s="5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="N58" s="5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" ht="15" customHeight="1">
+      <c r="A59" s="67" t="inlineStr">
+        <is>
+          <t>TOTALS</t>
+        </is>
+      </c>
+      <c r="B59" s="67" t="n"/>
+      <c r="C59" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" s="67" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="M59" s="67" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="N59" s="67" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A10:N10"/>
     <mergeCell ref="A29:N29"/>
     <mergeCell ref="A36:N36"/>
     <mergeCell ref="A44:N44"/>
     <mergeCell ref="A50:N50"/>
+    <mergeCell ref="A56:N56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10260,7 +10550,7 @@
         </is>
       </c>
       <c r="B1" s="26" t="n">
-        <v>581</v>
+        <v>540</v>
       </c>
     </row>
     <row r="2">
@@ -10280,7 +10570,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>26</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4">
@@ -10290,7 +10580,7 @@
         </is>
       </c>
       <c r="B4" s="26" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
@@ -10300,7 +10590,7 @@
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
@@ -10340,7 +10630,7 @@
         </is>
       </c>
       <c r="B9" s="26" t="n">
-        <v>370</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -10371,17 +10661,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>981 Spools</t>
+          <t>1019 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>30 Workable</t>
+          <t>185 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>30 Issued</t>
+          <t>187 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10434,7 +10724,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -10451,7 +10741,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -10471,7 +10761,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -10491,7 +10781,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -10543,7 +10833,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>0</v>
+        <v>5262.4</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -10626,17 +10916,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>981 Spools</t>
+          <t>1019 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>30 Workable</t>
+          <t>185 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>30 Issued</t>
+          <t>187 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10689,7 +10979,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -10706,7 +10996,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>507</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -10726,7 +11016,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>358</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -10746,7 +11036,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -10798,7 +11088,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>0</v>
+        <v>694</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -10857,17 +11147,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>981 Spools</t>
+          <t>1019 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>30 Workable</t>
+          <t>185 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>30 Issued</t>
+          <t>187 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10920,7 +11210,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -10937,7 +11227,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -10957,7 +11247,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -10977,7 +11267,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11029,7 +11319,7 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>0</v>
+        <v>4568.4</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0</v>
@@ -11134,7 +11424,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
@@ -11175,17 +11465,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>981 Spools</t>
+          <t>1019 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>30 Workable</t>
+          <t>185 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>30 Issued</t>
+          <t>187 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11246,7 +11536,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11269,7 +11559,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11295,7 +11585,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11321,7 +11611,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11347,7 +11637,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>0</v>
@@ -11376,7 +11666,7 @@
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
       <c r="E9" s="22" t="n">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="F9" s="5" t="n"/>
       <c r="G9" s="5" t="n"/>
@@ -11433,7 +11723,7 @@
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="22" t="n">
-        <v>370</v>
+        <v>126</v>
       </c>
       <c r="F12" s="5" t="n"/>
       <c r="G12" s="5" t="n"/>
@@ -11452,7 +11742,7 @@
       <c r="C13" s="30" t="n"/>
       <c r="D13" s="30" t="n"/>
       <c r="E13" s="28" t="n">
-        <v>581</v>
+        <v>18</v>
       </c>
       <c r="F13" s="5" t="n"/>
       <c r="G13" s="5" t="n"/>
@@ -11480,7 +11770,7 @@
         <v/>
       </c>
       <c r="E14" s="24" t="n">
-        <v>981</v>
+        <v>1019</v>
       </c>
       <c r="F14" s="23" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add schedules to weld types
</commit_message>
<xml_diff>
--- a/database/7052/JobSummary.xlsx
+++ b/database/7052/JobSummary.xlsx
@@ -4439,14 +4439,14 @@
       <c r="E1" s="49" t="n"/>
       <c r="F1" s="58" t="inlineStr">
         <is>
-          <t>185 Workable</t>
+          <t>264 Workable</t>
         </is>
       </c>
       <c r="G1" s="61" t="n"/>
       <c r="H1" s="49" t="n"/>
       <c r="I1" s="58" t="inlineStr">
         <is>
-          <t>187 Issued</t>
+          <t>264 Issued</t>
         </is>
       </c>
       <c r="J1" s="61" t="n"/>
@@ -5468,10 +5468,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>0</v>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="M33" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N33" s="1" t="inlineStr">
@@ -5513,7 +5513,7 @@
         <v>123</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>0</v>
@@ -5570,16 +5570,16 @@
         <v>5</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I35" s="1" t="n">
         <v>0</v>
@@ -5592,12 +5592,12 @@
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t>71.1%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="M35" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>62.2%</t>
         </is>
       </c>
       <c r="N35" s="1" t="inlineStr">
@@ -5621,19 +5621,19 @@
         <v>242</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>0</v>
@@ -5646,12 +5646,12 @@
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t>23.6%</t>
+          <t>31.8%</t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>10.7%</t>
         </is>
       </c>
       <c r="N36" s="1" t="inlineStr">
@@ -5675,7 +5675,7 @@
         <v>83</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>20</v>
@@ -5684,10 +5684,10 @@
         <v>63</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>0</v>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="M37" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>7.2%</t>
         </is>
       </c>
       <c r="N37" s="1" t="inlineStr">
@@ -5732,16 +5732,16 @@
         <v>61</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>0</v>
@@ -5754,12 +5754,12 @@
       </c>
       <c r="L38" s="1" t="inlineStr">
         <is>
-          <t>16.0%</t>
+          <t>18.1%</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.4%</t>
         </is>
       </c>
       <c r="N38" s="1" t="inlineStr">
@@ -5783,19 +5783,19 @@
         <v>42</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>0</v>
@@ -5808,12 +5808,12 @@
       </c>
       <c r="L39" s="1" t="inlineStr">
         <is>
-          <t>35.7%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="M39" s="1" t="inlineStr">
         <is>
-          <t>4.8%</t>
+          <t>23.8%</t>
         </is>
       </c>
       <c r="N39" s="1" t="inlineStr">
@@ -5840,16 +5840,16 @@
         <v>3</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>0</v>
@@ -5862,12 +5862,12 @@
       </c>
       <c r="L40" s="1" t="inlineStr">
         <is>
-          <t>9.5%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>19.0%</t>
         </is>
       </c>
       <c r="N40" s="1" t="inlineStr">
@@ -5894,16 +5894,16 @@
         <v>40</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G41" s="1" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>0</v>
@@ -5916,12 +5916,12 @@
       </c>
       <c r="L41" s="1" t="inlineStr">
         <is>
-          <t>8.3%</t>
+          <t>12.2%</t>
         </is>
       </c>
       <c r="M41" s="1" t="inlineStr">
         <is>
-          <t>6.4%</t>
+          <t>10.9%</t>
         </is>
       </c>
       <c r="N41" s="1" t="inlineStr">
@@ -5948,16 +5948,16 @@
         <v>4</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>0</v>
@@ -5970,12 +5970,12 @@
       </c>
       <c r="L42" s="1" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="M42" s="1" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="N42" s="1" t="inlineStr">
@@ -5999,7 +5999,7 @@
         <v>39</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>0</v>
@@ -6053,7 +6053,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>1</v>
@@ -6164,16 +6164,16 @@
         <v>0</v>
       </c>
       <c r="E46" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F46" s="1" t="n">
+      <c r="H46" s="1" t="n">
         <v>8</v>
-      </c>
-      <c r="G46" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" s="1" t="n">
-        <v>9</v>
       </c>
       <c r="I46" s="1" t="n">
         <v>0</v>
@@ -6186,12 +6186,12 @@
       </c>
       <c r="L46" s="1" t="inlineStr">
         <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="M46" s="1" t="inlineStr">
+        <is>
           <t>11.1%</t>
-        </is>
-      </c>
-      <c r="M46" s="1" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N46" s="1" t="inlineStr">
@@ -6215,19 +6215,19 @@
         <v>22</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E47" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G47" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F47" s="1" t="n">
+      <c r="H47" s="1" t="n">
         <v>17</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H47" s="1" t="n">
-        <v>20</v>
       </c>
       <c r="I47" s="1" t="n">
         <v>0</v>
@@ -6240,12 +6240,12 @@
       </c>
       <c r="L47" s="1" t="inlineStr">
         <is>
+          <t>68.2%</t>
+        </is>
+      </c>
+      <c r="M47" s="1" t="inlineStr">
+        <is>
           <t>22.7%</t>
-        </is>
-      </c>
-      <c r="M47" s="1" t="inlineStr">
-        <is>
-          <t>9.1%</t>
         </is>
       </c>
       <c r="N47" s="1" t="inlineStr">
@@ -6269,19 +6269,19 @@
         <v>25</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>0</v>
@@ -6294,12 +6294,12 @@
       </c>
       <c r="L48" s="1" t="inlineStr">
         <is>
-          <t>44.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>8.0%</t>
+          <t>36.0%</t>
         </is>
       </c>
       <c r="N48" s="1" t="inlineStr">
@@ -6323,19 +6323,19 @@
         <v>53</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E49" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="G49" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F49" s="1" t="n">
+      <c r="H49" s="1" t="n">
         <v>44</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H49" s="1" t="n">
-        <v>49</v>
       </c>
       <c r="I49" s="1" t="n">
         <v>0</v>
@@ -6348,12 +6348,12 @@
       </c>
       <c r="L49" s="1" t="inlineStr">
         <is>
+          <t>28.3%</t>
+        </is>
+      </c>
+      <c r="M49" s="1" t="inlineStr">
+        <is>
           <t>17.0%</t>
-        </is>
-      </c>
-      <c r="M49" s="1" t="inlineStr">
-        <is>
-          <t>7.5%</t>
         </is>
       </c>
       <c r="N49" s="1" t="inlineStr">
@@ -6425,19 +6425,19 @@
         <v>1019</v>
       </c>
       <c r="D51" s="64" t="n">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E51" s="64" t="n">
-        <v>185</v>
+        <v>264</v>
       </c>
       <c r="F51" s="64" t="n">
-        <v>834</v>
+        <v>755</v>
       </c>
       <c r="G51" s="64" t="n">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="H51" s="64" t="n">
-        <v>995</v>
+        <v>893</v>
       </c>
       <c r="I51" s="64" t="n">
         <v>0</v>
@@ -6450,12 +6450,12 @@
       </c>
       <c r="L51" s="64" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="M51" s="64" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="N51" s="64" t="inlineStr">
@@ -6489,7 +6489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -6523,96 +6523,6 @@
           <t>PM In Status Report (Not in Line List)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>44-2</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>48-1</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>52-2</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" s="1" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>341-1</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>401-1</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="1" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>401-2</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>401-3</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>401-4</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>463-4</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
-      <c r="D10" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6753,10 +6663,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>0</v>
@@ -6774,7 +6684,7 @@
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
@@ -6798,7 +6708,7 @@
         <v>123</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>0</v>
@@ -6855,16 +6765,16 @@
         <v>5</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
@@ -6877,12 +6787,12 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>71.1%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="M5" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>62.2%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
@@ -6906,19 +6816,19 @@
         <v>242</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -6931,12 +6841,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>23.6%</t>
+          <t>31.8%</t>
         </is>
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>10.7%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -6960,7 +6870,7 @@
         <v>83</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>20</v>
@@ -6969,10 +6879,10 @@
         <v>63</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I7" s="5" t="n">
         <v>0</v>
@@ -6990,7 +6900,7 @@
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>7.2%</t>
         </is>
       </c>
       <c r="N7" s="5" t="inlineStr">
@@ -7017,16 +6927,16 @@
         <v>61</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I8" s="5" t="n">
         <v>0</v>
@@ -7039,12 +6949,12 @@
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>16.0%</t>
+          <t>18.1%</t>
         </is>
       </c>
       <c r="M8" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.4%</t>
         </is>
       </c>
       <c r="N8" s="5" t="inlineStr">
@@ -7068,19 +6978,19 @@
         <v>42</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>0</v>
@@ -7093,12 +7003,12 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>35.7%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="M9" s="5" t="inlineStr">
         <is>
-          <t>4.8%</t>
+          <t>23.8%</t>
         </is>
       </c>
       <c r="N9" s="5" t="inlineStr">
@@ -7125,16 +7035,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5" t="n">
         <v>0</v>
@@ -7147,12 +7057,12 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>9.5%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="M10" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>19.0%</t>
         </is>
       </c>
       <c r="N10" s="5" t="inlineStr">
@@ -7179,16 +7089,16 @@
         <v>40</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I11" s="5" t="n">
         <v>0</v>
@@ -7201,12 +7111,12 @@
       </c>
       <c r="L11" s="5" t="inlineStr">
         <is>
-          <t>8.3%</t>
+          <t>12.2%</t>
         </is>
       </c>
       <c r="M11" s="5" t="inlineStr">
         <is>
-          <t>6.4%</t>
+          <t>10.9%</t>
         </is>
       </c>
       <c r="N11" s="5" t="inlineStr">
@@ -7233,16 +7143,16 @@
         <v>4</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
@@ -7255,12 +7165,12 @@
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="M12" s="5" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="N12" s="5" t="inlineStr">
@@ -7284,7 +7194,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>0</v>
@@ -7338,7 +7248,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>1</v>
@@ -7449,16 +7359,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="H16" s="5" t="n">
         <v>8</v>
-      </c>
-      <c r="G16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5" t="n">
-        <v>9</v>
       </c>
       <c r="I16" s="5" t="n">
         <v>0</v>
@@ -7471,12 +7381,12 @@
       </c>
       <c r="L16" s="5" t="inlineStr">
         <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="M16" s="5" t="inlineStr">
+        <is>
           <t>11.1%</t>
-        </is>
-      </c>
-      <c r="M16" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N16" s="5" t="inlineStr">
@@ -7500,19 +7410,19 @@
         <v>22</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E17" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G17" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="H17" s="5" t="n">
         <v>17</v>
-      </c>
-      <c r="G17" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H17" s="5" t="n">
-        <v>20</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -7525,12 +7435,12 @@
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
+          <t>68.2%</t>
+        </is>
+      </c>
+      <c r="M17" s="5" t="inlineStr">
+        <is>
           <t>22.7%</t>
-        </is>
-      </c>
-      <c r="M17" s="5" t="inlineStr">
-        <is>
-          <t>9.1%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -7554,19 +7464,19 @@
         <v>25</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I18" s="5" t="n">
         <v>0</v>
@@ -7579,12 +7489,12 @@
       </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
-          <t>44.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="M18" s="5" t="inlineStr">
         <is>
-          <t>8.0%</t>
+          <t>36.0%</t>
         </is>
       </c>
       <c r="N18" s="5" t="inlineStr">
@@ -7608,19 +7518,19 @@
         <v>53</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E19" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="G19" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="H19" s="5" t="n">
         <v>44</v>
-      </c>
-      <c r="G19" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H19" s="5" t="n">
-        <v>49</v>
       </c>
       <c r="I19" s="5" t="n">
         <v>0</v>
@@ -7633,12 +7543,12 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
+          <t>28.3%</t>
+        </is>
+      </c>
+      <c r="M19" s="5" t="inlineStr">
+        <is>
           <t>17.0%</t>
-        </is>
-      </c>
-      <c r="M19" s="5" t="inlineStr">
-        <is>
-          <t>7.5%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -7710,19 +7620,19 @@
         <v>1019</v>
       </c>
       <c r="D21" s="67" t="n">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E21" s="67" t="n">
-        <v>185</v>
+        <v>264</v>
       </c>
       <c r="F21" s="67" t="n">
-        <v>834</v>
+        <v>755</v>
       </c>
       <c r="G21" s="67" t="n">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="H21" s="67" t="n">
-        <v>995</v>
+        <v>893</v>
       </c>
       <c r="I21" s="67" t="n">
         <v>0</v>
@@ -7735,12 +7645,12 @@
       </c>
       <c r="L21" s="67" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="M21" s="67" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="N21" s="67" t="inlineStr">
@@ -7884,16 +7794,16 @@
         <v>36</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>0</v>
@@ -7906,12 +7816,12 @@
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>8.6%</t>
+          <t>12.5%</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>6.6%</t>
+          <t>11.2%</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
@@ -7938,16 +7848,16 @@
         <v>4</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>0</v>
@@ -7960,12 +7870,12 @@
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="M4" s="5" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="N4" s="5" t="inlineStr">
@@ -7992,16 +7902,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="H5" s="5" t="n">
         <v>9</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>11</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
@@ -8014,12 +7924,12 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
+          <t>76.9%</t>
+        </is>
+      </c>
+      <c r="M5" s="5" t="inlineStr">
+        <is>
           <t>30.8%</t>
-        </is>
-      </c>
-      <c r="M5" s="5" t="inlineStr">
-        <is>
-          <t>15.4%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
@@ -8046,16 +7956,16 @@
         <v>4</v>
       </c>
       <c r="E6" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="H6" s="5" t="n">
         <v>9</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>10</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -8068,12 +7978,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
+          <t>58.3%</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
           <t>25.0%</t>
-        </is>
-      </c>
-      <c r="M6" s="5" t="inlineStr">
-        <is>
-          <t>16.7%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -8106,10 +8016,10 @@
         <v>34</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I7" s="5" t="n">
         <v>0</v>
@@ -8127,7 +8037,7 @@
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>10.5%</t>
         </is>
       </c>
       <c r="N7" s="5" t="inlineStr">
@@ -8150,16 +8060,16 @@
         <v>52</v>
       </c>
       <c r="E8" s="67" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F8" s="67" t="n">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G8" s="67" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H8" s="67" t="n">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="I8" s="67" t="n">
         <v>0</v>
@@ -8172,12 +8082,12 @@
       </c>
       <c r="L8" s="67" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="M8" s="67" t="inlineStr">
         <is>
-          <t>6%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="N8" s="67" t="inlineStr">
@@ -8296,19 +8206,19 @@
         <v>10</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="G12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="5" t="n">
         <v>8</v>
-      </c>
-      <c r="G12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <v>10</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
@@ -8321,12 +8231,12 @@
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="M12" s="5" t="inlineStr">
+        <is>
           <t>20.0%</t>
-        </is>
-      </c>
-      <c r="M12" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N12" s="5" t="inlineStr">
@@ -8350,19 +8260,19 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" s="5" t="n">
         <v>7</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>12</v>
       </c>
       <c r="I13" s="5" t="n">
         <v>0</v>
@@ -8375,12 +8285,12 @@
       </c>
       <c r="L13" s="5" t="inlineStr">
         <is>
-          <t>58.3%</t>
+          <t>83.3%</t>
         </is>
       </c>
       <c r="M13" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>41.7%</t>
         </is>
       </c>
       <c r="N13" s="5" t="inlineStr">
@@ -8407,16 +8317,16 @@
         <v>0</v>
       </c>
       <c r="E14" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="H14" s="5" t="n">
         <v>21</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>26</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>0</v>
@@ -8429,12 +8339,12 @@
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
+          <t>46.4%</t>
+        </is>
+      </c>
+      <c r="M14" s="5" t="inlineStr">
+        <is>
           <t>25.0%</t>
-        </is>
-      </c>
-      <c r="M14" s="5" t="inlineStr">
-        <is>
-          <t>7.1%</t>
         </is>
       </c>
       <c r="N14" s="5" t="inlineStr">
@@ -8467,10 +8377,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I15" s="5" t="n">
         <v>0</v>
@@ -8488,7 +8398,7 @@
       </c>
       <c r="M15" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N15" s="5" t="inlineStr">
@@ -8515,16 +8425,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="H16" s="5" t="n">
         <v>8</v>
-      </c>
-      <c r="G16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5" t="n">
-        <v>9</v>
       </c>
       <c r="I16" s="5" t="n">
         <v>0</v>
@@ -8537,12 +8447,12 @@
       </c>
       <c r="L16" s="5" t="inlineStr">
         <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="M16" s="5" t="inlineStr">
+        <is>
           <t>11.1%</t>
-        </is>
-      </c>
-      <c r="M16" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N16" s="5" t="inlineStr">
@@ -8569,16 +8479,16 @@
         <v>5</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -8591,12 +8501,12 @@
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
-          <t>71.1%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="M17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>62.2%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -8672,19 +8582,19 @@
         <v>204</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="I19" s="5" t="n">
         <v>0</v>
@@ -8697,12 +8607,12 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>26.0%</t>
+          <t>35.8%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
         <is>
-          <t>1.5%</t>
+          <t>10.8%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -8726,7 +8636,7 @@
         <v>73</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>20</v>
@@ -8735,10 +8645,10 @@
         <v>53</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I20" s="5" t="n">
         <v>0</v>
@@ -8756,7 +8666,7 @@
       </c>
       <c r="M20" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>8.2%</t>
         </is>
       </c>
       <c r="N20" s="5" t="inlineStr">
@@ -8783,16 +8693,16 @@
         <v>33</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I21" s="5" t="n">
         <v>0</v>
@@ -8805,12 +8715,12 @@
       </c>
       <c r="L21" s="5" t="inlineStr">
         <is>
-          <t>22.7%</t>
+          <t>25.8%</t>
         </is>
       </c>
       <c r="M21" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>9.1%</t>
         </is>
       </c>
       <c r="N21" s="5" t="inlineStr">
@@ -8837,16 +8747,16 @@
         <v>0</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I22" s="5" t="n">
         <v>0</v>
@@ -8859,12 +8769,12 @@
       </c>
       <c r="L22" s="5" t="inlineStr">
         <is>
-          <t>70.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="M22" s="5" t="inlineStr">
         <is>
-          <t>10.0%</t>
+          <t>45.0%</t>
         </is>
       </c>
       <c r="N22" s="5" t="inlineStr">
@@ -8891,16 +8801,16 @@
         <v>3</v>
       </c>
       <c r="E23" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G23" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="H23" s="5" t="n">
         <v>10</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>11</v>
       </c>
       <c r="I23" s="5" t="n">
         <v>0</v>
@@ -8913,12 +8823,12 @@
       </c>
       <c r="L23" s="5" t="inlineStr">
         <is>
+          <t>27.3%</t>
+        </is>
+      </c>
+      <c r="M23" s="5" t="inlineStr">
+        <is>
           <t>9.1%</t>
-        </is>
-      </c>
-      <c r="M23" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N23" s="5" t="inlineStr">
@@ -8996,7 +8906,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>1</v>
@@ -9100,19 +9010,19 @@
         <v>506</v>
       </c>
       <c r="D27" s="67" t="n">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E27" s="67" t="n">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="F27" s="67" t="n">
-        <v>350</v>
+        <v>302</v>
       </c>
       <c r="G27" s="67" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="H27" s="67" t="n">
-        <v>499</v>
+        <v>416</v>
       </c>
       <c r="I27" s="67" t="n">
         <v>0</v>
@@ -9125,12 +9035,12 @@
       </c>
       <c r="L27" s="67" t="inlineStr">
         <is>
-          <t>31%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="M27" s="67" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="N27" s="67" t="inlineStr">
@@ -9306,16 +9216,16 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G32" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I32" s="5" t="n">
         <v>0</v>
@@ -9328,12 +9238,12 @@
       </c>
       <c r="L32" s="5" t="inlineStr">
         <is>
-          <t>10.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="M32" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>30.0%</t>
         </is>
       </c>
       <c r="N32" s="5" t="inlineStr">
@@ -9357,19 +9267,19 @@
         <v>12</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E33" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F33" s="5" t="n">
+      <c r="H33" s="5" t="n">
         <v>11</v>
-      </c>
-      <c r="G33" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="5" t="n">
-        <v>12</v>
       </c>
       <c r="I33" s="5" t="n">
         <v>0</v>
@@ -9382,12 +9292,12 @@
       </c>
       <c r="L33" s="5" t="inlineStr">
         <is>
+          <t>66.7%</t>
+        </is>
+      </c>
+      <c r="M33" s="5" t="inlineStr">
+        <is>
           <t>8.3%</t>
-        </is>
-      </c>
-      <c r="M33" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
       <c r="N33" s="5" t="inlineStr">
@@ -9407,19 +9317,19 @@
         <v>26</v>
       </c>
       <c r="D34" s="67" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E34" s="67" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F34" s="67" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G34" s="67" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H34" s="67" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I34" s="67" t="n">
         <v>0</v>
@@ -9432,12 +9342,12 @@
       </c>
       <c r="L34" s="67" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="M34" s="67" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="N34" s="67" t="inlineStr">
@@ -9556,7 +9466,7 @@
         <v>122</v>
       </c>
       <c r="D38" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>0</v>
@@ -9610,7 +9520,7 @@
         <v>17</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>0</v>
@@ -9718,7 +9628,7 @@
         <v>35</v>
       </c>
       <c r="D41" s="5" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>0</v>
@@ -9768,7 +9678,7 @@
         <v>177</v>
       </c>
       <c r="D42" s="67" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E42" s="67" t="n">
         <v>0</v>
@@ -10079,7 +9989,7 @@
     <row r="50" ht="37" customHeight="1">
       <c r="A50" s="65" t="inlineStr">
         <is>
-          <t>#N/A Summary</t>
+          <t>Galv. Summary</t>
         </is>
       </c>
     </row>
@@ -10423,7 +10333,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>0</v>
@@ -10473,7 +10383,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="67" t="n">
         <v>0</v>
@@ -10550,7 +10460,7 @@
         </is>
       </c>
       <c r="B1" s="26" t="n">
-        <v>540</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2">
@@ -10570,7 +10480,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>124</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -10580,7 +10490,7 @@
         </is>
       </c>
       <c r="B4" s="26" t="n">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
@@ -10590,7 +10500,7 @@
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>24</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6">
@@ -10630,7 +10540,7 @@
         </is>
       </c>
       <c r="B9" s="26" t="n">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -10666,12 +10576,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>185 Workable</t>
+          <t>264 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>187 Issued</t>
+          <t>264 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10724,7 +10634,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -10741,7 +10651,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>875</v>
+        <v>767</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -10761,7 +10671,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>450</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -10781,7 +10691,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -10833,7 +10743,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>5262.4</v>
+        <v>4515.799999999999</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -10921,12 +10831,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>185 Workable</t>
+          <t>264 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>187 Issued</t>
+          <t>264 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10979,7 +10889,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>137</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -10996,7 +10906,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>507</v>
+        <v>734</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11016,7 +10926,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>358</v>
+        <v>83</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11036,7 +10946,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11088,7 +10998,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>694</v>
+        <v>2393.6</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -11152,12 +11062,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>185 Workable</t>
+          <t>264 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>187 Issued</t>
+          <t>264 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11227,7 +11137,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>368</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11247,7 +11157,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11267,7 +11177,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11319,7 +11229,7 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>4568.4</v>
+        <v>2122.2</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0</v>
@@ -11424,7 +11334,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
@@ -11470,12 +11380,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>185 Workable</t>
+          <t>264 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>187 Issued</t>
+          <t>264 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11536,7 +11446,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>124</v>
+        <v>28</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11559,7 +11469,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11585,7 +11495,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11611,7 +11521,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11637,7 +11547,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>0</v>
@@ -11666,7 +11576,7 @@
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
       <c r="E9" s="22" t="n">
-        <v>187</v>
+        <v>264</v>
       </c>
       <c r="F9" s="5" t="n"/>
       <c r="G9" s="5" t="n"/>
@@ -11723,7 +11633,7 @@
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="22" t="n">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="F12" s="5" t="n"/>
       <c r="G12" s="5" t="n"/>
@@ -11742,7 +11652,7 @@
       <c r="C13" s="30" t="n"/>
       <c r="D13" s="30" t="n"/>
       <c r="E13" s="28" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F13" s="5" t="n"/>
       <c r="G13" s="5" t="n"/>

</xml_diff>

<commit_message>
Fix discrep issue and workable fc issue
</commit_message>
<xml_diff>
--- a/database/7052/JobSummary.xlsx
+++ b/database/7052/JobSummary.xlsx
@@ -4439,14 +4439,14 @@
       <c r="E1" s="49" t="n"/>
       <c r="F1" s="58" t="inlineStr">
         <is>
-          <t>264 Workable</t>
+          <t>412 Workable</t>
         </is>
       </c>
       <c r="G1" s="61" t="n"/>
       <c r="H1" s="49" t="n"/>
       <c r="I1" s="58" t="inlineStr">
         <is>
-          <t>264 Issued</t>
+          <t>417 Issued</t>
         </is>
       </c>
       <c r="J1" s="61" t="n"/>
@@ -5570,16 +5570,16 @@
         <v>5</v>
       </c>
       <c r="E35" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="F35" s="1" t="n">
+      <c r="H35" s="1" t="n">
         <v>12</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v>17</v>
       </c>
       <c r="I35" s="1" t="n">
         <v>0</v>
@@ -5592,12 +5592,12 @@
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
+          <t>82.2%</t>
+        </is>
+      </c>
+      <c r="M35" s="1" t="inlineStr">
+        <is>
           <t>73.3%</t>
-        </is>
-      </c>
-      <c r="M35" s="1" t="inlineStr">
-        <is>
-          <t>62.2%</t>
         </is>
       </c>
       <c r="N35" s="1" t="inlineStr">
@@ -5624,16 +5624,16 @@
         <v>80</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>0</v>
@@ -5646,12 +5646,12 @@
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t>31.8%</t>
+          <t>50.8%</t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>10.7%</t>
+          <t>13.2%</t>
         </is>
       </c>
       <c r="N36" s="1" t="inlineStr">
@@ -5678,10 +5678,10 @@
         <v>50</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>6</v>
@@ -5700,7 +5700,7 @@
       </c>
       <c r="L37" s="1" t="inlineStr">
         <is>
-          <t>24.1%</t>
+          <t>22.9%</t>
         </is>
       </c>
       <c r="M37" s="1" t="inlineStr">
@@ -5732,10 +5732,10 @@
         <v>61</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>6</v>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="L38" s="1" t="inlineStr">
         <is>
-          <t>18.1%</t>
+          <t>20.2%</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
@@ -5792,10 +5792,10 @@
         <v>18</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>0</v>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="M39" s="1" t="inlineStr">
         <is>
-          <t>23.8%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="N39" s="1" t="inlineStr">
@@ -5840,16 +5840,16 @@
         <v>3</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>0</v>
@@ -5862,12 +5862,12 @@
       </c>
       <c r="L40" s="1" t="inlineStr">
         <is>
-          <t>52.4%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>19.0%</t>
+          <t>42.9%</t>
         </is>
       </c>
       <c r="N40" s="1" t="inlineStr">
@@ -5894,10 +5894,10 @@
         <v>40</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>17</v>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="L41" s="1" t="inlineStr">
         <is>
-          <t>12.2%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="M41" s="1" t="inlineStr">
@@ -5948,10 +5948,10 @@
         <v>4</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>2</v>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="L42" s="1" t="inlineStr">
         <is>
-          <t>4.8%</t>
+          <t>47.6%</t>
         </is>
       </c>
       <c r="M42" s="1" t="inlineStr">
@@ -6002,10 +6002,10 @@
         <v>24</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>0</v>
@@ -6024,7 +6024,7 @@
       </c>
       <c r="L43" s="1" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5.1%</t>
         </is>
       </c>
       <c r="M43" s="1" t="inlineStr">
@@ -6056,10 +6056,10 @@
         <v>6</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>0</v>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="L44" s="1" t="inlineStr">
         <is>
-          <t>10.0%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M44" s="1" t="inlineStr">
@@ -6170,10 +6170,10 @@
         <v>2</v>
       </c>
       <c r="G46" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I46" s="1" t="n">
         <v>0</v>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="M46" s="1" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>22.2%</t>
         </is>
       </c>
       <c r="N46" s="1" t="inlineStr">
@@ -6218,16 +6218,16 @@
         <v>6</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I47" s="1" t="n">
         <v>0</v>
@@ -6240,12 +6240,12 @@
       </c>
       <c r="L47" s="1" t="inlineStr">
         <is>
-          <t>68.2%</t>
+          <t>72.7%</t>
         </is>
       </c>
       <c r="M47" s="1" t="inlineStr">
         <is>
-          <t>22.7%</t>
+          <t>27.3%</t>
         </is>
       </c>
       <c r="N47" s="1" t="inlineStr">
@@ -6272,16 +6272,16 @@
         <v>4</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>0</v>
@@ -6294,12 +6294,12 @@
       </c>
       <c r="L48" s="1" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>84.0%</t>
         </is>
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>36.0%</t>
+          <t>56.0%</t>
         </is>
       </c>
       <c r="N48" s="1" t="inlineStr">
@@ -6326,10 +6326,10 @@
         <v>6</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G49" s="1" t="n">
         <v>9</v>
@@ -6348,7 +6348,7 @@
       </c>
       <c r="L49" s="1" t="inlineStr">
         <is>
-          <t>28.3%</t>
+          <t>37.7%</t>
         </is>
       </c>
       <c r="M49" s="1" t="inlineStr">
@@ -6428,16 +6428,16 @@
         <v>300</v>
       </c>
       <c r="E51" s="64" t="n">
-        <v>264</v>
+        <v>413</v>
       </c>
       <c r="F51" s="64" t="n">
-        <v>755</v>
+        <v>606</v>
       </c>
       <c r="G51" s="64" t="n">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="H51" s="64" t="n">
-        <v>893</v>
+        <v>859</v>
       </c>
       <c r="I51" s="64" t="n">
         <v>0</v>
@@ -6450,12 +6450,12 @@
       </c>
       <c r="L51" s="64" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="M51" s="64" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="N51" s="64" t="inlineStr">
@@ -6489,7 +6489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -6523,6 +6523,1236 @@
           <t>PM In Status Report (Not in Line List)</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>19-1</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>20-1</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>46-1</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>56-1</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>98-1</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>99-6</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>100-1</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>201-2</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>201-3</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>201-4</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>201-5</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>201-6</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>201-7</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>201-8</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
+      <c r="D15" s="1" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>201-9</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>201-10</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>202-1</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="n"/>
+      <c r="D18" s="1" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>202-2</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="n"/>
+      <c r="C19" s="1" t="n"/>
+      <c r="D19" s="1" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>202-3</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>202-4</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>202-5</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="1" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>202-6</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>202-7</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>210-2</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="1" t="n"/>
+      <c r="D25" s="1" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>223-1</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>223-2</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="n"/>
+      <c r="D27" s="1" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>223-3</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="1" t="n"/>
+      <c r="D28" s="1" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>224-1</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>224-2</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>224-3</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="n"/>
+      <c r="C31" s="1" t="n"/>
+      <c r="D31" s="1" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>225-1</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="n"/>
+      <c r="C32" s="1" t="n"/>
+      <c r="D32" s="1" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>225-2</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="n"/>
+      <c r="C33" s="1" t="n"/>
+      <c r="D33" s="1" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>225-3</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="n"/>
+      <c r="C34" s="1" t="n"/>
+      <c r="D34" s="1" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>226-1</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="n"/>
+      <c r="C35" s="1" t="n"/>
+      <c r="D35" s="1" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>226-2</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="n"/>
+      <c r="C36" s="1" t="n"/>
+      <c r="D36" s="1" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>226-3</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="n"/>
+      <c r="C37" s="1" t="n"/>
+      <c r="D37" s="1" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>227-1</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="n"/>
+      <c r="C38" s="1" t="n"/>
+      <c r="D38" s="1" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>227-2</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="n"/>
+      <c r="C39" s="1" t="n"/>
+      <c r="D39" s="1" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>227-3</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="n"/>
+      <c r="C40" s="1" t="n"/>
+      <c r="D40" s="1" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>228-1</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="n"/>
+      <c r="C41" s="1" t="n"/>
+      <c r="D41" s="1" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>228-2</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="1" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>228-3</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="n"/>
+      <c r="C43" s="1" t="n"/>
+      <c r="D43" s="1" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>229-1</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="n"/>
+      <c r="C44" s="1" t="n"/>
+      <c r="D44" s="1" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>229-2</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="n"/>
+      <c r="C45" s="1" t="n"/>
+      <c r="D45" s="1" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>229-3</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="n"/>
+      <c r="C46" s="1" t="n"/>
+      <c r="D46" s="1" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>230-1</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="n"/>
+      <c r="C47" s="1" t="n"/>
+      <c r="D47" s="1" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>230-2</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="n"/>
+      <c r="C48" s="1" t="n"/>
+      <c r="D48" s="1" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>230-3</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="n"/>
+      <c r="C49" s="1" t="n"/>
+      <c r="D49" s="1" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>231-1</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="n"/>
+      <c r="C50" s="1" t="n"/>
+      <c r="D50" s="1" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>231-2</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="n"/>
+      <c r="C51" s="1" t="n"/>
+      <c r="D51" s="1" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>231-3</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="n"/>
+      <c r="C52" s="1" t="n"/>
+      <c r="D52" s="1" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>232-1</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="n"/>
+      <c r="C53" s="1" t="n"/>
+      <c r="D53" s="1" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>232-2</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="n"/>
+      <c r="C54" s="1" t="n"/>
+      <c r="D54" s="1" t="n"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>232-3</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="n"/>
+      <c r="C55" s="1" t="n"/>
+      <c r="D55" s="1" t="n"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>233-1</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="n"/>
+      <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>233-2</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="n"/>
+      <c r="C57" s="1" t="n"/>
+      <c r="D57" s="1" t="n"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>233-3</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="n"/>
+      <c r="C58" s="1" t="n"/>
+      <c r="D58" s="1" t="n"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>234-1</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="n"/>
+      <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>234-2</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="n"/>
+      <c r="C60" s="1" t="n"/>
+      <c r="D60" s="1" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>234-3</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="n"/>
+      <c r="C61" s="1" t="n"/>
+      <c r="D61" s="1" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>235-1</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="n"/>
+      <c r="D62" s="1" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>236-1</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="n"/>
+      <c r="C63" s="1" t="n"/>
+      <c r="D63" s="1" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>236-2</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="n"/>
+      <c r="D64" s="1" t="n"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>238-1</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="n"/>
+      <c r="C65" s="1" t="n"/>
+      <c r="D65" s="1" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>238-2</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="n"/>
+      <c r="C66" s="1" t="n"/>
+      <c r="D66" s="1" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>308-2</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="n"/>
+      <c r="C67" s="1" t="n"/>
+      <c r="D67" s="1" t="n"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>313-1</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="n"/>
+      <c r="C68" s="1" t="n"/>
+      <c r="D68" s="1" t="n"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>313-2</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="n"/>
+      <c r="C69" s="1" t="n"/>
+      <c r="D69" s="1" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>313-3</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="n"/>
+      <c r="C70" s="1" t="n"/>
+      <c r="D70" s="1" t="n"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>313-4</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="n"/>
+      <c r="C71" s="1" t="n"/>
+      <c r="D71" s="1" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>313-5</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="n"/>
+      <c r="C72" s="1" t="n"/>
+      <c r="D72" s="1" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>314-1</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="n"/>
+      <c r="C73" s="1" t="n"/>
+      <c r="D73" s="1" t="n"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>314-2</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="n"/>
+      <c r="C74" s="1" t="n"/>
+      <c r="D74" s="1" t="n"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>314-3</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="n"/>
+      <c r="C75" s="1" t="n"/>
+      <c r="D75" s="1" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>319-1</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="n"/>
+      <c r="C76" s="1" t="n"/>
+      <c r="D76" s="1" t="n"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>325-1</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="n"/>
+      <c r="C77" s="1" t="n"/>
+      <c r="D77" s="1" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>325-2</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="n"/>
+      <c r="C78" s="1" t="n"/>
+      <c r="D78" s="1" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>326-1</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="n"/>
+      <c r="C79" s="1" t="n"/>
+      <c r="D79" s="1" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>326-2</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="n"/>
+      <c r="C80" s="1" t="n"/>
+      <c r="D80" s="1" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>333-1</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="n"/>
+      <c r="C81" s="1" t="n"/>
+      <c r="D81" s="1" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>335-1</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="n"/>
+      <c r="C82" s="1" t="n"/>
+      <c r="D82" s="1" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>336-1</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="n"/>
+      <c r="C83" s="1" t="n"/>
+      <c r="D83" s="1" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>336-2</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="n"/>
+      <c r="C84" s="1" t="n"/>
+      <c r="D84" s="1" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>337-1</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="n"/>
+      <c r="C85" s="1" t="n"/>
+      <c r="D85" s="1" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>337-2</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="n"/>
+      <c r="C86" s="1" t="n"/>
+      <c r="D86" s="1" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>338-1</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="n"/>
+      <c r="C87" s="1" t="n"/>
+      <c r="D87" s="1" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>339-1</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="n"/>
+      <c r="C88" s="1" t="n"/>
+      <c r="D88" s="1" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>339-2</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="n"/>
+      <c r="C89" s="1" t="n"/>
+      <c r="D89" s="1" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>343-1</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="n"/>
+      <c r="C90" s="1" t="n"/>
+      <c r="D90" s="1" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>343-2</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="n"/>
+      <c r="C91" s="1" t="n"/>
+      <c r="D91" s="1" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>344-1</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="n"/>
+      <c r="C92" s="1" t="n"/>
+      <c r="D92" s="1" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>344-2</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="n"/>
+      <c r="C93" s="1" t="n"/>
+      <c r="D93" s="1" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>345-1</t>
+        </is>
+      </c>
+      <c r="B94" s="1" t="n"/>
+      <c r="C94" s="1" t="n"/>
+      <c r="D94" s="1" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>358-1</t>
+        </is>
+      </c>
+      <c r="B95" s="1" t="n"/>
+      <c r="C95" s="1" t="n"/>
+      <c r="D95" s="1" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>399-1</t>
+        </is>
+      </c>
+      <c r="B96" s="1" t="n"/>
+      <c r="C96" s="1" t="n"/>
+      <c r="D96" s="1" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>401-5</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="n"/>
+      <c r="C97" s="1" t="n"/>
+      <c r="D97" s="1" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>401-6</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="n"/>
+      <c r="C98" s="1" t="n"/>
+      <c r="D98" s="1" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>402-1</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="n"/>
+      <c r="C99" s="1" t="n"/>
+      <c r="D99" s="1" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>402-2</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="n"/>
+      <c r="C100" s="1" t="n"/>
+      <c r="D100" s="1" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>402-3</t>
+        </is>
+      </c>
+      <c r="B101" s="1" t="n"/>
+      <c r="C101" s="1" t="n"/>
+      <c r="D101" s="1" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>403-1</t>
+        </is>
+      </c>
+      <c r="B102" s="1" t="n"/>
+      <c r="C102" s="1" t="n"/>
+      <c r="D102" s="1" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>403-2</t>
+        </is>
+      </c>
+      <c r="B103" s="1" t="n"/>
+      <c r="C103" s="1" t="n"/>
+      <c r="D103" s="1" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>403-3</t>
+        </is>
+      </c>
+      <c r="B104" s="1" t="n"/>
+      <c r="C104" s="1" t="n"/>
+      <c r="D104" s="1" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>403-4</t>
+        </is>
+      </c>
+      <c r="B105" s="1" t="n"/>
+      <c r="C105" s="1" t="n"/>
+      <c r="D105" s="1" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>403-5</t>
+        </is>
+      </c>
+      <c r="B106" s="1" t="n"/>
+      <c r="C106" s="1" t="n"/>
+      <c r="D106" s="1" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>404-1</t>
+        </is>
+      </c>
+      <c r="B107" s="1" t="n"/>
+      <c r="C107" s="1" t="n"/>
+      <c r="D107" s="1" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>404-2</t>
+        </is>
+      </c>
+      <c r="B108" s="1" t="n"/>
+      <c r="C108" s="1" t="n"/>
+      <c r="D108" s="1" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>404-3</t>
+        </is>
+      </c>
+      <c r="B109" s="1" t="n"/>
+      <c r="C109" s="1" t="n"/>
+      <c r="D109" s="1" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>404-4</t>
+        </is>
+      </c>
+      <c r="B110" s="1" t="n"/>
+      <c r="C110" s="1" t="n"/>
+      <c r="D110" s="1" t="n"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>404-5</t>
+        </is>
+      </c>
+      <c r="B111" s="1" t="n"/>
+      <c r="C111" s="1" t="n"/>
+      <c r="D111" s="1" t="n"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>405-1</t>
+        </is>
+      </c>
+      <c r="B112" s="1" t="n"/>
+      <c r="C112" s="1" t="n"/>
+      <c r="D112" s="1" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>405-2</t>
+        </is>
+      </c>
+      <c r="B113" s="1" t="n"/>
+      <c r="C113" s="1" t="n"/>
+      <c r="D113" s="1" t="n"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>405-3</t>
+        </is>
+      </c>
+      <c r="B114" s="1" t="n"/>
+      <c r="C114" s="1" t="n"/>
+      <c r="D114" s="1" t="n"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>405-4</t>
+        </is>
+      </c>
+      <c r="B115" s="1" t="n"/>
+      <c r="C115" s="1" t="n"/>
+      <c r="D115" s="1" t="n"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>406-1</t>
+        </is>
+      </c>
+      <c r="B116" s="1" t="n"/>
+      <c r="C116" s="1" t="n"/>
+      <c r="D116" s="1" t="n"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>406-2</t>
+        </is>
+      </c>
+      <c r="B117" s="1" t="n"/>
+      <c r="C117" s="1" t="n"/>
+      <c r="D117" s="1" t="n"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>406-3</t>
+        </is>
+      </c>
+      <c r="B118" s="1" t="n"/>
+      <c r="C118" s="1" t="n"/>
+      <c r="D118" s="1" t="n"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>406-4</t>
+        </is>
+      </c>
+      <c r="B119" s="1" t="n"/>
+      <c r="C119" s="1" t="n"/>
+      <c r="D119" s="1" t="n"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>407-1</t>
+        </is>
+      </c>
+      <c r="B120" s="1" t="n"/>
+      <c r="C120" s="1" t="n"/>
+      <c r="D120" s="1" t="n"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>407-2</t>
+        </is>
+      </c>
+      <c r="B121" s="1" t="n"/>
+      <c r="C121" s="1" t="n"/>
+      <c r="D121" s="1" t="n"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>407-3</t>
+        </is>
+      </c>
+      <c r="B122" s="1" t="n"/>
+      <c r="C122" s="1" t="n"/>
+      <c r="D122" s="1" t="n"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>407-4</t>
+        </is>
+      </c>
+      <c r="B123" s="1" t="n"/>
+      <c r="C123" s="1" t="n"/>
+      <c r="D123" s="1" t="n"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>407-5</t>
+        </is>
+      </c>
+      <c r="B124" s="1" t="n"/>
+      <c r="C124" s="1" t="n"/>
+      <c r="D124" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6765,16 +7995,16 @@
         <v>5</v>
       </c>
       <c r="E5" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="H5" s="5" t="n">
         <v>12</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>17</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
@@ -6787,12 +8017,12 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
+          <t>82.2%</t>
+        </is>
+      </c>
+      <c r="M5" s="5" t="inlineStr">
+        <is>
           <t>73.3%</t>
-        </is>
-      </c>
-      <c r="M5" s="5" t="inlineStr">
-        <is>
-          <t>62.2%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
@@ -6819,16 +8049,16 @@
         <v>80</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -6841,12 +8071,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>31.8%</t>
+          <t>50.8%</t>
         </is>
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>10.7%</t>
+          <t>13.2%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -6873,10 +8103,10 @@
         <v>50</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>6</v>
@@ -6895,7 +8125,7 @@
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>24.1%</t>
+          <t>22.9%</t>
         </is>
       </c>
       <c r="M7" s="5" t="inlineStr">
@@ -6927,10 +8157,10 @@
         <v>61</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>6</v>
@@ -6949,7 +8179,7 @@
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>18.1%</t>
+          <t>20.2%</t>
         </is>
       </c>
       <c r="M8" s="5" t="inlineStr">
@@ -6987,10 +8217,10 @@
         <v>18</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>0</v>
@@ -7008,7 +8238,7 @@
       </c>
       <c r="M9" s="5" t="inlineStr">
         <is>
-          <t>23.8%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="N9" s="5" t="inlineStr">
@@ -7035,16 +8265,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I10" s="5" t="n">
         <v>0</v>
@@ -7057,12 +8287,12 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>52.4%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="M10" s="5" t="inlineStr">
         <is>
-          <t>19.0%</t>
+          <t>42.9%</t>
         </is>
       </c>
       <c r="N10" s="5" t="inlineStr">
@@ -7089,10 +8319,10 @@
         <v>40</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>17</v>
@@ -7111,7 +8341,7 @@
       </c>
       <c r="L11" s="5" t="inlineStr">
         <is>
-          <t>12.2%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="M11" s="5" t="inlineStr">
@@ -7143,10 +8373,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>2</v>
@@ -7165,7 +8395,7 @@
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
-          <t>4.8%</t>
+          <t>47.6%</t>
         </is>
       </c>
       <c r="M12" s="5" t="inlineStr">
@@ -7197,10 +8427,10 @@
         <v>24</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>0</v>
@@ -7219,7 +8449,7 @@
       </c>
       <c r="L13" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5.1%</t>
         </is>
       </c>
       <c r="M13" s="5" t="inlineStr">
@@ -7251,10 +8481,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
@@ -7273,7 +8503,7 @@
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>10.0%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M14" s="5" t="inlineStr">
@@ -7365,10 +8595,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="5" t="n">
         <v>0</v>
@@ -7386,7 +8616,7 @@
       </c>
       <c r="M16" s="5" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>22.2%</t>
         </is>
       </c>
       <c r="N16" s="5" t="inlineStr">
@@ -7413,16 +8643,16 @@
         <v>6</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -7435,12 +8665,12 @@
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
-          <t>68.2%</t>
+          <t>72.7%</t>
         </is>
       </c>
       <c r="M17" s="5" t="inlineStr">
         <is>
-          <t>22.7%</t>
+          <t>27.3%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -7467,16 +8697,16 @@
         <v>4</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I18" s="5" t="n">
         <v>0</v>
@@ -7489,12 +8719,12 @@
       </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>84.0%</t>
         </is>
       </c>
       <c r="M18" s="5" t="inlineStr">
         <is>
-          <t>36.0%</t>
+          <t>56.0%</t>
         </is>
       </c>
       <c r="N18" s="5" t="inlineStr">
@@ -7521,10 +8751,10 @@
         <v>6</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>9</v>
@@ -7543,7 +8773,7 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>28.3%</t>
+          <t>37.7%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
@@ -7623,16 +8853,16 @@
         <v>300</v>
       </c>
       <c r="E21" s="67" t="n">
-        <v>264</v>
+        <v>412</v>
       </c>
       <c r="F21" s="67" t="n">
-        <v>755</v>
+        <v>607</v>
       </c>
       <c r="G21" s="67" t="n">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="H21" s="67" t="n">
-        <v>893</v>
+        <v>859</v>
       </c>
       <c r="I21" s="67" t="n">
         <v>0</v>
@@ -7645,12 +8875,12 @@
       </c>
       <c r="L21" s="67" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="M21" s="67" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="N21" s="67" t="inlineStr">
@@ -7794,10 +9024,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>17</v>
@@ -7816,7 +9046,7 @@
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>12.5%</t>
+          <t>58.6%</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
@@ -7848,10 +9078,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>2</v>
@@ -7870,7 +9100,7 @@
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
-          <t>4.8%</t>
+          <t>47.6%</t>
         </is>
       </c>
       <c r="M4" s="5" t="inlineStr">
@@ -7902,16 +9132,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
@@ -7924,12 +9154,12 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>76.9%</t>
+          <t>84.6%</t>
         </is>
       </c>
       <c r="M5" s="5" t="inlineStr">
         <is>
-          <t>30.8%</t>
+          <t>61.5%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
@@ -7956,16 +9186,16 @@
         <v>4</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -7978,12 +9208,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>58.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>25.0%</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -8010,10 +9240,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>4</v>
@@ -8032,7 +9262,7 @@
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>10.5%</t>
+          <t>84.2%</t>
         </is>
       </c>
       <c r="M7" s="5" t="inlineStr">
@@ -8060,16 +9290,16 @@
         <v>52</v>
       </c>
       <c r="E8" s="67" t="n">
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="F8" s="67" t="n">
-        <v>215</v>
+        <v>97</v>
       </c>
       <c r="G8" s="67" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H8" s="67" t="n">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I8" s="67" t="n">
         <v>0</v>
@@ -8082,12 +9312,12 @@
       </c>
       <c r="L8" s="67" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="M8" s="67" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="N8" s="67" t="inlineStr">
@@ -8269,10 +9499,10 @@
         <v>2</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I13" s="5" t="n">
         <v>0</v>
@@ -8290,7 +9520,7 @@
       </c>
       <c r="M13" s="5" t="inlineStr">
         <is>
-          <t>41.7%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="N13" s="5" t="inlineStr">
@@ -8317,10 +9547,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>7</v>
@@ -8339,7 +9569,7 @@
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>46.4%</t>
+          <t>64.3%</t>
         </is>
       </c>
       <c r="M14" s="5" t="inlineStr">
@@ -8431,10 +9661,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="5" t="n">
         <v>0</v>
@@ -8452,7 +9682,7 @@
       </c>
       <c r="M16" s="5" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>22.2%</t>
         </is>
       </c>
       <c r="N16" s="5" t="inlineStr">
@@ -8479,16 +9709,16 @@
         <v>5</v>
       </c>
       <c r="E17" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="H17" s="5" t="n">
         <v>12</v>
-      </c>
-      <c r="G17" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="H17" s="5" t="n">
-        <v>17</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -8501,12 +9731,12 @@
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
+          <t>82.2%</t>
+        </is>
+      </c>
+      <c r="M17" s="5" t="inlineStr">
+        <is>
           <t>73.3%</t>
-        </is>
-      </c>
-      <c r="M17" s="5" t="inlineStr">
-        <is>
-          <t>62.2%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -8585,16 +9815,16 @@
         <v>74</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="I19" s="5" t="n">
         <v>0</v>
@@ -8607,12 +9837,12 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>35.8%</t>
+          <t>44.6%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
         <is>
-          <t>10.8%</t>
+          <t>13.7%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -8639,10 +9869,10 @@
         <v>40</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>6</v>
@@ -8661,7 +9891,7 @@
       </c>
       <c r="L20" s="5" t="inlineStr">
         <is>
-          <t>27.4%</t>
+          <t>26.0%</t>
         </is>
       </c>
       <c r="M20" s="5" t="inlineStr">
@@ -8693,10 +9923,10 @@
         <v>33</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G21" s="5" t="n">
         <v>6</v>
@@ -8715,7 +9945,7 @@
       </c>
       <c r="L21" s="5" t="inlineStr">
         <is>
-          <t>25.8%</t>
+          <t>28.8%</t>
         </is>
       </c>
       <c r="M21" s="5" t="inlineStr">
@@ -8753,10 +9983,10 @@
         <v>4</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I22" s="5" t="n">
         <v>0</v>
@@ -8774,7 +10004,7 @@
       </c>
       <c r="M22" s="5" t="inlineStr">
         <is>
-          <t>45.0%</t>
+          <t>65.0%</t>
         </is>
       </c>
       <c r="N22" s="5" t="inlineStr">
@@ -8801,16 +10031,16 @@
         <v>3</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I23" s="5" t="n">
         <v>0</v>
@@ -8823,12 +10053,12 @@
       </c>
       <c r="L23" s="5" t="inlineStr">
         <is>
-          <t>27.3%</t>
+          <t>36.4%</t>
         </is>
       </c>
       <c r="M23" s="5" t="inlineStr">
         <is>
-          <t>9.1%</t>
+          <t>18.2%</t>
         </is>
       </c>
       <c r="N23" s="5" t="inlineStr">
@@ -8909,10 +10139,10 @@
         <v>6</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G25" s="5" t="n">
         <v>0</v>
@@ -8931,7 +10161,7 @@
       </c>
       <c r="L25" s="5" t="inlineStr">
         <is>
-          <t>10.0%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M25" s="5" t="inlineStr">
@@ -8963,10 +10193,10 @@
         <v>2</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>0</v>
@@ -8985,7 +10215,7 @@
       </c>
       <c r="L26" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="M26" s="5" t="inlineStr">
@@ -9013,16 +10243,16 @@
         <v>178</v>
       </c>
       <c r="E27" s="67" t="n">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="F27" s="67" t="n">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="G27" s="67" t="n">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="H27" s="67" t="n">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="I27" s="67" t="n">
         <v>0</v>
@@ -9035,12 +10265,12 @@
       </c>
       <c r="L27" s="67" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>46%</t>
         </is>
       </c>
       <c r="M27" s="67" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="N27" s="67" t="inlineStr">
@@ -9222,10 +10452,10 @@
         <v>2</v>
       </c>
       <c r="G32" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H32" s="5" t="n">
         <v>3</v>
-      </c>
-      <c r="H32" s="5" t="n">
-        <v>7</v>
       </c>
       <c r="I32" s="5" t="n">
         <v>0</v>
@@ -9243,7 +10473,7 @@
       </c>
       <c r="M32" s="5" t="inlineStr">
         <is>
-          <t>30.0%</t>
+          <t>70.0%</t>
         </is>
       </c>
       <c r="N32" s="5" t="inlineStr">
@@ -9276,10 +10506,10 @@
         <v>4</v>
       </c>
       <c r="G33" s="5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I33" s="5" t="n">
         <v>0</v>
@@ -9297,7 +10527,7 @@
       </c>
       <c r="M33" s="5" t="inlineStr">
         <is>
-          <t>8.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="N33" s="5" t="inlineStr">
@@ -9326,10 +10556,10 @@
         <v>8</v>
       </c>
       <c r="G34" s="67" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H34" s="67" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I34" s="67" t="n">
         <v>0</v>
@@ -9347,7 +10577,7 @@
       </c>
       <c r="M34" s="67" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="N34" s="67" t="inlineStr">
@@ -10460,7 +11690,7 @@
         </is>
       </c>
       <c r="B1" s="26" t="n">
-        <v>461</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2">
@@ -10470,7 +11700,7 @@
         </is>
       </c>
       <c r="B2" s="26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -10480,7 +11710,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>55</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4">
@@ -10490,7 +11720,7 @@
         </is>
       </c>
       <c r="B4" s="26" t="n">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -10500,7 +11730,7 @@
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
@@ -10540,7 +11770,7 @@
         </is>
       </c>
       <c r="B9" s="26" t="n">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -10576,12 +11806,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>264 Workable</t>
+          <t>412 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>264 Issued</t>
+          <t>417 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10651,7 +11881,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>767</v>
+        <v>456</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -10671,7 +11901,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -10743,7 +11973,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>4515.799999999999</v>
+        <v>3198.2</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -10831,12 +12061,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>264 Workable</t>
+          <t>412 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>264 Issued</t>
+          <t>417 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10906,7 +12136,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>734</v>
+        <v>423</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -10926,7 +12156,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -10998,7 +12228,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>2393.6</v>
+        <v>1245</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -11062,12 +12292,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>264 Workable</t>
+          <t>412 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>264 Issued</t>
+          <t>417 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11229,7 +12459,7 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>2122.2</v>
+        <v>1953.2</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0</v>
@@ -11334,7 +12564,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
@@ -11380,12 +12610,12 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>264 Workable</t>
+          <t>412 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>264 Issued</t>
+          <t>417 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11469,7 +12699,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>343</v>
+        <v>290</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11495,7 +12725,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>223</v>
+        <v>95</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11521,7 +12751,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11576,7 +12806,7 @@
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
       <c r="E9" s="22" t="n">
-        <v>264</v>
+        <v>417</v>
       </c>
       <c r="F9" s="5" t="n"/>
       <c r="G9" s="5" t="n"/>
@@ -11595,7 +12825,7 @@
       <c r="C10" s="5" t="n"/>
       <c r="D10" s="5" t="n"/>
       <c r="E10" s="22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="5" t="n"/>
       <c r="G10" s="5" t="n"/>
@@ -11633,7 +12863,7 @@
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="22" t="n">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="F12" s="5" t="n"/>
       <c r="G12" s="5" t="n"/>
@@ -11652,7 +12882,7 @@
       <c r="C13" s="30" t="n"/>
       <c r="D13" s="30" t="n"/>
       <c r="E13" s="28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5" t="n"/>
       <c r="G13" s="5" t="n"/>

</xml_diff>

<commit_message>
Assign schedules and classes to welds
</commit_message>
<xml_diff>
--- a/database/7052/JobSummary.xlsx
+++ b/database/7052/JobSummary.xlsx
@@ -4439,7 +4439,7 @@
       <c r="E1" s="49" t="n"/>
       <c r="F1" s="58" t="inlineStr">
         <is>
-          <t>412 Workable</t>
+          <t>437 Workable</t>
         </is>
       </c>
       <c r="G1" s="61" t="n"/>
@@ -5474,7 +5474,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J33" s="1" t="n">
         <v>0</v>
@@ -5567,13 +5567,13 @@
         <v>45</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>33</v>
@@ -5582,7 +5582,7 @@
         <v>12</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J35" s="1" t="n">
         <v>0</v>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t>82.2%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="M35" s="1" t="inlineStr">
@@ -5621,22 +5621,22 @@
         <v>242</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J36" s="1" t="n">
         <v>0</v>
@@ -5646,12 +5646,12 @@
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t>50.8%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>13.2%</t>
+          <t>14.5%</t>
         </is>
       </c>
       <c r="N36" s="1" t="inlineStr">
@@ -5675,7 +5675,7 @@
         <v>83</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>19</v>
@@ -5684,13 +5684,13 @@
         <v>64</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J37" s="1" t="n">
         <v>0</v>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="M37" s="1" t="inlineStr">
         <is>
-          <t>7.2%</t>
+          <t>13.3%</t>
         </is>
       </c>
       <c r="N37" s="1" t="inlineStr">
@@ -5729,7 +5729,7 @@
         <v>94</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>19</v>
@@ -5738,13 +5738,13 @@
         <v>75</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>0</v>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="M38" s="1" t="inlineStr">
         <is>
-          <t>6.4%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="N38" s="1" t="inlineStr">
@@ -5786,19 +5786,19 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G39" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="H39" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="G39" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>21</v>
-      </c>
       <c r="I39" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J39" s="1" t="n">
         <v>0</v>
@@ -5808,12 +5808,12 @@
       </c>
       <c r="L39" s="1" t="inlineStr">
         <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="M39" s="1" t="inlineStr">
+        <is>
           <t>57.1%</t>
-        </is>
-      </c>
-      <c r="M39" s="1" t="inlineStr">
-        <is>
-          <t>50.0%</t>
         </is>
       </c>
       <c r="N39" s="1" t="inlineStr">
@@ -5837,22 +5837,22 @@
         <v>21</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J40" s="1" t="n">
         <v>0</v>
@@ -5862,12 +5862,12 @@
       </c>
       <c r="L40" s="1" t="inlineStr">
         <is>
-          <t>57.1%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>42.9%</t>
+          <t>47.6%</t>
         </is>
       </c>
       <c r="N40" s="1" t="inlineStr">
@@ -5894,10 +5894,10 @@
         <v>40</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>17</v>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="L41" s="1" t="inlineStr">
         <is>
-          <t>57.1%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="M41" s="1" t="inlineStr">
@@ -5948,10 +5948,10 @@
         <v>4</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>2</v>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="L42" s="1" t="inlineStr">
         <is>
-          <t>47.6%</t>
+          <t>59.5%</t>
         </is>
       </c>
       <c r="M42" s="1" t="inlineStr">
@@ -6053,7 +6053,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>0</v>
@@ -6161,7 +6161,7 @@
         <v>9</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>7</v>
@@ -6176,7 +6176,7 @@
         <v>7</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="1" t="n">
         <v>0</v>
@@ -6224,10 +6224,10 @@
         <v>6</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I47" s="1" t="n">
         <v>0</v>
@@ -6245,7 +6245,7 @@
       </c>
       <c r="M47" s="1" t="inlineStr">
         <is>
-          <t>27.3%</t>
+          <t>54.5%</t>
         </is>
       </c>
       <c r="N47" s="1" t="inlineStr">
@@ -6278,13 +6278,13 @@
         <v>4</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J48" s="1" t="n">
         <v>0</v>
@@ -6299,7 +6299,7 @@
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>56.0%</t>
+          <t>64.0%</t>
         </is>
       </c>
       <c r="N48" s="1" t="inlineStr">
@@ -6323,22 +6323,22 @@
         <v>53</v>
       </c>
       <c r="D49" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="I49" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="E49" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="F49" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="H49" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="I49" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="J49" s="1" t="n">
         <v>0</v>
@@ -6348,12 +6348,12 @@
       </c>
       <c r="L49" s="1" t="inlineStr">
         <is>
-          <t>37.7%</t>
+          <t>43.4%</t>
         </is>
       </c>
       <c r="M49" s="1" t="inlineStr">
         <is>
-          <t>17.0%</t>
+          <t>20.8%</t>
         </is>
       </c>
       <c r="N49" s="1" t="inlineStr">
@@ -6425,22 +6425,22 @@
         <v>1019</v>
       </c>
       <c r="D51" s="64" t="n">
-        <v>300</v>
+        <v>385</v>
       </c>
       <c r="E51" s="64" t="n">
-        <v>413</v>
+        <v>470</v>
       </c>
       <c r="F51" s="64" t="n">
-        <v>606</v>
+        <v>549</v>
       </c>
       <c r="G51" s="64" t="n">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="H51" s="64" t="n">
-        <v>859</v>
+        <v>830</v>
       </c>
       <c r="I51" s="64" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="J51" s="64" t="n">
         <v>0</v>
@@ -6450,12 +6450,12 @@
       </c>
       <c r="L51" s="64" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>43%</t>
         </is>
       </c>
       <c r="M51" s="64" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>19%</t>
         </is>
       </c>
       <c r="N51" s="64" t="inlineStr">
@@ -6489,7 +6489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -6523,1236 +6523,6 @@
           <t>PM In Status Report (Not in Line List)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>19-1</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>20-1</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>46-1</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" s="1" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>56-1</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>98-1</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="1" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>99-6</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>100-1</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>201-2</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>201-3</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
-      <c r="D10" s="1" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>201-4</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
-      <c r="D11" s="1" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>201-5</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="n"/>
-      <c r="D12" s="1" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>201-6</t>
-        </is>
-      </c>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
-      <c r="D13" s="1" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>201-7</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="n"/>
-      <c r="D14" s="1" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>201-8</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="n"/>
-      <c r="D15" s="1" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>201-9</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
-      <c r="D16" s="1" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>201-10</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="n"/>
-      <c r="D17" s="1" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>202-1</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>202-2</t>
-        </is>
-      </c>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
-      <c r="D19" s="1" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>202-3</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
-      <c r="D20" s="1" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>202-4</t>
-        </is>
-      </c>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>202-5</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="n"/>
-      <c r="D22" s="1" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>202-6</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="n"/>
-      <c r="C23" s="1" t="n"/>
-      <c r="D23" s="1" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>202-7</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="n"/>
-      <c r="D24" s="1" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>210-2</t>
-        </is>
-      </c>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>223-1</t>
-        </is>
-      </c>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
-      <c r="D26" s="1" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>223-2</t>
-        </is>
-      </c>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="n"/>
-      <c r="D27" s="1" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>223-3</t>
-        </is>
-      </c>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="n"/>
-      <c r="D28" s="1" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>224-1</t>
-        </is>
-      </c>
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="n"/>
-      <c r="D29" s="1" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>224-2</t>
-        </is>
-      </c>
-      <c r="B30" s="1" t="n"/>
-      <c r="C30" s="1" t="n"/>
-      <c r="D30" s="1" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>224-3</t>
-        </is>
-      </c>
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="n"/>
-      <c r="D31" s="1" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>225-1</t>
-        </is>
-      </c>
-      <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="n"/>
-      <c r="D32" s="1" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>225-2</t>
-        </is>
-      </c>
-      <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="n"/>
-      <c r="D33" s="1" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>225-3</t>
-        </is>
-      </c>
-      <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="n"/>
-      <c r="D34" s="1" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>226-1</t>
-        </is>
-      </c>
-      <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="n"/>
-      <c r="D35" s="1" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>226-2</t>
-        </is>
-      </c>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="n"/>
-      <c r="D36" s="1" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>226-3</t>
-        </is>
-      </c>
-      <c r="B37" s="1" t="n"/>
-      <c r="C37" s="1" t="n"/>
-      <c r="D37" s="1" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>227-1</t>
-        </is>
-      </c>
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="1" t="n"/>
-      <c r="D38" s="1" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>227-2</t>
-        </is>
-      </c>
-      <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="n"/>
-      <c r="D39" s="1" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>227-3</t>
-        </is>
-      </c>
-      <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="n"/>
-      <c r="D40" s="1" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>228-1</t>
-        </is>
-      </c>
-      <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="n"/>
-      <c r="D41" s="1" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>228-2</t>
-        </is>
-      </c>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="n"/>
-      <c r="D42" s="1" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>228-3</t>
-        </is>
-      </c>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="n"/>
-      <c r="D43" s="1" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>229-1</t>
-        </is>
-      </c>
-      <c r="B44" s="1" t="n"/>
-      <c r="C44" s="1" t="n"/>
-      <c r="D44" s="1" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>229-2</t>
-        </is>
-      </c>
-      <c r="B45" s="1" t="n"/>
-      <c r="C45" s="1" t="n"/>
-      <c r="D45" s="1" t="n"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>229-3</t>
-        </is>
-      </c>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="n"/>
-      <c r="D46" s="1" t="n"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>230-1</t>
-        </is>
-      </c>
-      <c r="B47" s="1" t="n"/>
-      <c r="C47" s="1" t="n"/>
-      <c r="D47" s="1" t="n"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>230-2</t>
-        </is>
-      </c>
-      <c r="B48" s="1" t="n"/>
-      <c r="C48" s="1" t="n"/>
-      <c r="D48" s="1" t="n"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>230-3</t>
-        </is>
-      </c>
-      <c r="B49" s="1" t="n"/>
-      <c r="C49" s="1" t="n"/>
-      <c r="D49" s="1" t="n"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>231-1</t>
-        </is>
-      </c>
-      <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="n"/>
-      <c r="D50" s="1" t="n"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>231-2</t>
-        </is>
-      </c>
-      <c r="B51" s="1" t="n"/>
-      <c r="C51" s="1" t="n"/>
-      <c r="D51" s="1" t="n"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>231-3</t>
-        </is>
-      </c>
-      <c r="B52" s="1" t="n"/>
-      <c r="C52" s="1" t="n"/>
-      <c r="D52" s="1" t="n"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>232-1</t>
-        </is>
-      </c>
-      <c r="B53" s="1" t="n"/>
-      <c r="C53" s="1" t="n"/>
-      <c r="D53" s="1" t="n"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>232-2</t>
-        </is>
-      </c>
-      <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="n"/>
-      <c r="D54" s="1" t="n"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>232-3</t>
-        </is>
-      </c>
-      <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="n"/>
-      <c r="D55" s="1" t="n"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>233-1</t>
-        </is>
-      </c>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="n"/>
-      <c r="D56" s="1" t="n"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>233-2</t>
-        </is>
-      </c>
-      <c r="B57" s="1" t="n"/>
-      <c r="C57" s="1" t="n"/>
-      <c r="D57" s="1" t="n"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>233-3</t>
-        </is>
-      </c>
-      <c r="B58" s="1" t="n"/>
-      <c r="C58" s="1" t="n"/>
-      <c r="D58" s="1" t="n"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>234-1</t>
-        </is>
-      </c>
-      <c r="B59" s="1" t="n"/>
-      <c r="C59" s="1" t="n"/>
-      <c r="D59" s="1" t="n"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>234-2</t>
-        </is>
-      </c>
-      <c r="B60" s="1" t="n"/>
-      <c r="C60" s="1" t="n"/>
-      <c r="D60" s="1" t="n"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>234-3</t>
-        </is>
-      </c>
-      <c r="B61" s="1" t="n"/>
-      <c r="C61" s="1" t="n"/>
-      <c r="D61" s="1" t="n"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>235-1</t>
-        </is>
-      </c>
-      <c r="B62" s="1" t="n"/>
-      <c r="C62" s="1" t="n"/>
-      <c r="D62" s="1" t="n"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>236-1</t>
-        </is>
-      </c>
-      <c r="B63" s="1" t="n"/>
-      <c r="C63" s="1" t="n"/>
-      <c r="D63" s="1" t="n"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>236-2</t>
-        </is>
-      </c>
-      <c r="B64" s="1" t="n"/>
-      <c r="C64" s="1" t="n"/>
-      <c r="D64" s="1" t="n"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>238-1</t>
-        </is>
-      </c>
-      <c r="B65" s="1" t="n"/>
-      <c r="C65" s="1" t="n"/>
-      <c r="D65" s="1" t="n"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>238-2</t>
-        </is>
-      </c>
-      <c r="B66" s="1" t="n"/>
-      <c r="C66" s="1" t="n"/>
-      <c r="D66" s="1" t="n"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>308-2</t>
-        </is>
-      </c>
-      <c r="B67" s="1" t="n"/>
-      <c r="C67" s="1" t="n"/>
-      <c r="D67" s="1" t="n"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>313-1</t>
-        </is>
-      </c>
-      <c r="B68" s="1" t="n"/>
-      <c r="C68" s="1" t="n"/>
-      <c r="D68" s="1" t="n"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>313-2</t>
-        </is>
-      </c>
-      <c r="B69" s="1" t="n"/>
-      <c r="C69" s="1" t="n"/>
-      <c r="D69" s="1" t="n"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>313-3</t>
-        </is>
-      </c>
-      <c r="B70" s="1" t="n"/>
-      <c r="C70" s="1" t="n"/>
-      <c r="D70" s="1" t="n"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>313-4</t>
-        </is>
-      </c>
-      <c r="B71" s="1" t="n"/>
-      <c r="C71" s="1" t="n"/>
-      <c r="D71" s="1" t="n"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>313-5</t>
-        </is>
-      </c>
-      <c r="B72" s="1" t="n"/>
-      <c r="C72" s="1" t="n"/>
-      <c r="D72" s="1" t="n"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>314-1</t>
-        </is>
-      </c>
-      <c r="B73" s="1" t="n"/>
-      <c r="C73" s="1" t="n"/>
-      <c r="D73" s="1" t="n"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>314-2</t>
-        </is>
-      </c>
-      <c r="B74" s="1" t="n"/>
-      <c r="C74" s="1" t="n"/>
-      <c r="D74" s="1" t="n"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>314-3</t>
-        </is>
-      </c>
-      <c r="B75" s="1" t="n"/>
-      <c r="C75" s="1" t="n"/>
-      <c r="D75" s="1" t="n"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>319-1</t>
-        </is>
-      </c>
-      <c r="B76" s="1" t="n"/>
-      <c r="C76" s="1" t="n"/>
-      <c r="D76" s="1" t="n"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>325-1</t>
-        </is>
-      </c>
-      <c r="B77" s="1" t="n"/>
-      <c r="C77" s="1" t="n"/>
-      <c r="D77" s="1" t="n"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>325-2</t>
-        </is>
-      </c>
-      <c r="B78" s="1" t="n"/>
-      <c r="C78" s="1" t="n"/>
-      <c r="D78" s="1" t="n"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>326-1</t>
-        </is>
-      </c>
-      <c r="B79" s="1" t="n"/>
-      <c r="C79" s="1" t="n"/>
-      <c r="D79" s="1" t="n"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>326-2</t>
-        </is>
-      </c>
-      <c r="B80" s="1" t="n"/>
-      <c r="C80" s="1" t="n"/>
-      <c r="D80" s="1" t="n"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>333-1</t>
-        </is>
-      </c>
-      <c r="B81" s="1" t="n"/>
-      <c r="C81" s="1" t="n"/>
-      <c r="D81" s="1" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>335-1</t>
-        </is>
-      </c>
-      <c r="B82" s="1" t="n"/>
-      <c r="C82" s="1" t="n"/>
-      <c r="D82" s="1" t="n"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>336-1</t>
-        </is>
-      </c>
-      <c r="B83" s="1" t="n"/>
-      <c r="C83" s="1" t="n"/>
-      <c r="D83" s="1" t="n"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>336-2</t>
-        </is>
-      </c>
-      <c r="B84" s="1" t="n"/>
-      <c r="C84" s="1" t="n"/>
-      <c r="D84" s="1" t="n"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>337-1</t>
-        </is>
-      </c>
-      <c r="B85" s="1" t="n"/>
-      <c r="C85" s="1" t="n"/>
-      <c r="D85" s="1" t="n"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>337-2</t>
-        </is>
-      </c>
-      <c r="B86" s="1" t="n"/>
-      <c r="C86" s="1" t="n"/>
-      <c r="D86" s="1" t="n"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>338-1</t>
-        </is>
-      </c>
-      <c r="B87" s="1" t="n"/>
-      <c r="C87" s="1" t="n"/>
-      <c r="D87" s="1" t="n"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>339-1</t>
-        </is>
-      </c>
-      <c r="B88" s="1" t="n"/>
-      <c r="C88" s="1" t="n"/>
-      <c r="D88" s="1" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="inlineStr">
-        <is>
-          <t>339-2</t>
-        </is>
-      </c>
-      <c r="B89" s="1" t="n"/>
-      <c r="C89" s="1" t="n"/>
-      <c r="D89" s="1" t="n"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>343-1</t>
-        </is>
-      </c>
-      <c r="B90" s="1" t="n"/>
-      <c r="C90" s="1" t="n"/>
-      <c r="D90" s="1" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="inlineStr">
-        <is>
-          <t>343-2</t>
-        </is>
-      </c>
-      <c r="B91" s="1" t="n"/>
-      <c r="C91" s="1" t="n"/>
-      <c r="D91" s="1" t="n"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>344-1</t>
-        </is>
-      </c>
-      <c r="B92" s="1" t="n"/>
-      <c r="C92" s="1" t="n"/>
-      <c r="D92" s="1" t="n"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="inlineStr">
-        <is>
-          <t>344-2</t>
-        </is>
-      </c>
-      <c r="B93" s="1" t="n"/>
-      <c r="C93" s="1" t="n"/>
-      <c r="D93" s="1" t="n"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>345-1</t>
-        </is>
-      </c>
-      <c r="B94" s="1" t="n"/>
-      <c r="C94" s="1" t="n"/>
-      <c r="D94" s="1" t="n"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="inlineStr">
-        <is>
-          <t>358-1</t>
-        </is>
-      </c>
-      <c r="B95" s="1" t="n"/>
-      <c r="C95" s="1" t="n"/>
-      <c r="D95" s="1" t="n"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="inlineStr">
-        <is>
-          <t>399-1</t>
-        </is>
-      </c>
-      <c r="B96" s="1" t="n"/>
-      <c r="C96" s="1" t="n"/>
-      <c r="D96" s="1" t="n"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="inlineStr">
-        <is>
-          <t>401-5</t>
-        </is>
-      </c>
-      <c r="B97" s="1" t="n"/>
-      <c r="C97" s="1" t="n"/>
-      <c r="D97" s="1" t="n"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>401-6</t>
-        </is>
-      </c>
-      <c r="B98" s="1" t="n"/>
-      <c r="C98" s="1" t="n"/>
-      <c r="D98" s="1" t="n"/>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="inlineStr">
-        <is>
-          <t>402-1</t>
-        </is>
-      </c>
-      <c r="B99" s="1" t="n"/>
-      <c r="C99" s="1" t="n"/>
-      <c r="D99" s="1" t="n"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="inlineStr">
-        <is>
-          <t>402-2</t>
-        </is>
-      </c>
-      <c r="B100" s="1" t="n"/>
-      <c r="C100" s="1" t="n"/>
-      <c r="D100" s="1" t="n"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="inlineStr">
-        <is>
-          <t>402-3</t>
-        </is>
-      </c>
-      <c r="B101" s="1" t="n"/>
-      <c r="C101" s="1" t="n"/>
-      <c r="D101" s="1" t="n"/>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="inlineStr">
-        <is>
-          <t>403-1</t>
-        </is>
-      </c>
-      <c r="B102" s="1" t="n"/>
-      <c r="C102" s="1" t="n"/>
-      <c r="D102" s="1" t="n"/>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="inlineStr">
-        <is>
-          <t>403-2</t>
-        </is>
-      </c>
-      <c r="B103" s="1" t="n"/>
-      <c r="C103" s="1" t="n"/>
-      <c r="D103" s="1" t="n"/>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="inlineStr">
-        <is>
-          <t>403-3</t>
-        </is>
-      </c>
-      <c r="B104" s="1" t="n"/>
-      <c r="C104" s="1" t="n"/>
-      <c r="D104" s="1" t="n"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="inlineStr">
-        <is>
-          <t>403-4</t>
-        </is>
-      </c>
-      <c r="B105" s="1" t="n"/>
-      <c r="C105" s="1" t="n"/>
-      <c r="D105" s="1" t="n"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="inlineStr">
-        <is>
-          <t>403-5</t>
-        </is>
-      </c>
-      <c r="B106" s="1" t="n"/>
-      <c r="C106" s="1" t="n"/>
-      <c r="D106" s="1" t="n"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="inlineStr">
-        <is>
-          <t>404-1</t>
-        </is>
-      </c>
-      <c r="B107" s="1" t="n"/>
-      <c r="C107" s="1" t="n"/>
-      <c r="D107" s="1" t="n"/>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="inlineStr">
-        <is>
-          <t>404-2</t>
-        </is>
-      </c>
-      <c r="B108" s="1" t="n"/>
-      <c r="C108" s="1" t="n"/>
-      <c r="D108" s="1" t="n"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="inlineStr">
-        <is>
-          <t>404-3</t>
-        </is>
-      </c>
-      <c r="B109" s="1" t="n"/>
-      <c r="C109" s="1" t="n"/>
-      <c r="D109" s="1" t="n"/>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="inlineStr">
-        <is>
-          <t>404-4</t>
-        </is>
-      </c>
-      <c r="B110" s="1" t="n"/>
-      <c r="C110" s="1" t="n"/>
-      <c r="D110" s="1" t="n"/>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="inlineStr">
-        <is>
-          <t>404-5</t>
-        </is>
-      </c>
-      <c r="B111" s="1" t="n"/>
-      <c r="C111" s="1" t="n"/>
-      <c r="D111" s="1" t="n"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>405-1</t>
-        </is>
-      </c>
-      <c r="B112" s="1" t="n"/>
-      <c r="C112" s="1" t="n"/>
-      <c r="D112" s="1" t="n"/>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="inlineStr">
-        <is>
-          <t>405-2</t>
-        </is>
-      </c>
-      <c r="B113" s="1" t="n"/>
-      <c r="C113" s="1" t="n"/>
-      <c r="D113" s="1" t="n"/>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="inlineStr">
-        <is>
-          <t>405-3</t>
-        </is>
-      </c>
-      <c r="B114" s="1" t="n"/>
-      <c r="C114" s="1" t="n"/>
-      <c r="D114" s="1" t="n"/>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="inlineStr">
-        <is>
-          <t>405-4</t>
-        </is>
-      </c>
-      <c r="B115" s="1" t="n"/>
-      <c r="C115" s="1" t="n"/>
-      <c r="D115" s="1" t="n"/>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="inlineStr">
-        <is>
-          <t>406-1</t>
-        </is>
-      </c>
-      <c r="B116" s="1" t="n"/>
-      <c r="C116" s="1" t="n"/>
-      <c r="D116" s="1" t="n"/>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="inlineStr">
-        <is>
-          <t>406-2</t>
-        </is>
-      </c>
-      <c r="B117" s="1" t="n"/>
-      <c r="C117" s="1" t="n"/>
-      <c r="D117" s="1" t="n"/>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="inlineStr">
-        <is>
-          <t>406-3</t>
-        </is>
-      </c>
-      <c r="B118" s="1" t="n"/>
-      <c r="C118" s="1" t="n"/>
-      <c r="D118" s="1" t="n"/>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="inlineStr">
-        <is>
-          <t>406-4</t>
-        </is>
-      </c>
-      <c r="B119" s="1" t="n"/>
-      <c r="C119" s="1" t="n"/>
-      <c r="D119" s="1" t="n"/>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t>407-1</t>
-        </is>
-      </c>
-      <c r="B120" s="1" t="n"/>
-      <c r="C120" s="1" t="n"/>
-      <c r="D120" s="1" t="n"/>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="inlineStr">
-        <is>
-          <t>407-2</t>
-        </is>
-      </c>
-      <c r="B121" s="1" t="n"/>
-      <c r="C121" s="1" t="n"/>
-      <c r="D121" s="1" t="n"/>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="inlineStr">
-        <is>
-          <t>407-3</t>
-        </is>
-      </c>
-      <c r="B122" s="1" t="n"/>
-      <c r="C122" s="1" t="n"/>
-      <c r="D122" s="1" t="n"/>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="inlineStr">
-        <is>
-          <t>407-4</t>
-        </is>
-      </c>
-      <c r="B123" s="1" t="n"/>
-      <c r="C123" s="1" t="n"/>
-      <c r="D123" s="1" t="n"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="inlineStr">
-        <is>
-          <t>407-5</t>
-        </is>
-      </c>
-      <c r="B124" s="1" t="n"/>
-      <c r="C124" s="1" t="n"/>
-      <c r="D124" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7899,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J3" s="5" t="n">
         <v>0</v>
@@ -7992,13 +6762,13 @@
         <v>45</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>33</v>
@@ -8007,7 +6777,7 @@
         <v>12</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J5" s="5" t="n">
         <v>0</v>
@@ -8017,7 +6787,7 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>82.2%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="M5" s="5" t="inlineStr">
@@ -8046,22 +6816,22 @@
         <v>242</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
@@ -8071,12 +6841,12 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>50.8%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>13.2%</t>
+          <t>14.5%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -8100,7 +6870,7 @@
         <v>83</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>19</v>
@@ -8109,13 +6879,13 @@
         <v>64</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J7" s="5" t="n">
         <v>0</v>
@@ -8130,7 +6900,7 @@
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>7.2%</t>
+          <t>13.3%</t>
         </is>
       </c>
       <c r="N7" s="5" t="inlineStr">
@@ -8154,7 +6924,7 @@
         <v>94</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>19</v>
@@ -8163,13 +6933,13 @@
         <v>75</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>0</v>
@@ -8184,7 +6954,7 @@
       </c>
       <c r="M8" s="5" t="inlineStr">
         <is>
-          <t>6.4%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="N8" s="5" t="inlineStr">
@@ -8211,19 +6981,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="H9" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="G9" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>21</v>
-      </c>
       <c r="I9" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J9" s="5" t="n">
         <v>0</v>
@@ -8233,12 +7003,12 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="M9" s="5" t="inlineStr">
+        <is>
           <t>57.1%</t>
-        </is>
-      </c>
-      <c r="M9" s="5" t="inlineStr">
-        <is>
-          <t>50.0%</t>
         </is>
       </c>
       <c r="N9" s="5" t="inlineStr">
@@ -8262,22 +7032,22 @@
         <v>21</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="5" t="n">
         <v>0</v>
@@ -8287,12 +7057,12 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>57.1%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="M10" s="5" t="inlineStr">
         <is>
-          <t>42.9%</t>
+          <t>47.6%</t>
         </is>
       </c>
       <c r="N10" s="5" t="inlineStr">
@@ -8319,10 +7089,10 @@
         <v>40</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>17</v>
@@ -8341,7 +7111,7 @@
       </c>
       <c r="L11" s="5" t="inlineStr">
         <is>
-          <t>57.1%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="M11" s="5" t="inlineStr">
@@ -8373,10 +7143,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>2</v>
@@ -8395,7 +7165,7 @@
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
-          <t>47.6%</t>
+          <t>59.5%</t>
         </is>
       </c>
       <c r="M12" s="5" t="inlineStr">
@@ -8478,7 +7248,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>0</v>
@@ -8586,7 +7356,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>7</v>
@@ -8601,7 +7371,7 @@
         <v>7</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>0</v>
@@ -8649,10 +7419,10 @@
         <v>6</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -8670,7 +7440,7 @@
       </c>
       <c r="M17" s="5" t="inlineStr">
         <is>
-          <t>27.3%</t>
+          <t>54.5%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -8703,13 +7473,13 @@
         <v>4</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J18" s="5" t="n">
         <v>0</v>
@@ -8724,7 +7494,7 @@
       </c>
       <c r="M18" s="5" t="inlineStr">
         <is>
-          <t>56.0%</t>
+          <t>64.0%</t>
         </is>
       </c>
       <c r="N18" s="5" t="inlineStr">
@@ -8748,22 +7518,22 @@
         <v>53</v>
       </c>
       <c r="D19" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="I19" s="5" t="n">
         <v>6</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="G19" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="H19" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="I19" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>0</v>
@@ -8773,12 +7543,12 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>37.7%</t>
+          <t>43.4%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
         <is>
-          <t>17.0%</t>
+          <t>20.8%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -8850,22 +7620,22 @@
         <v>1019</v>
       </c>
       <c r="D21" s="67" t="n">
-        <v>300</v>
+        <v>385</v>
       </c>
       <c r="E21" s="67" t="n">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="F21" s="67" t="n">
-        <v>607</v>
+        <v>582</v>
       </c>
       <c r="G21" s="67" t="n">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="H21" s="67" t="n">
-        <v>859</v>
+        <v>830</v>
       </c>
       <c r="I21" s="67" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="J21" s="67" t="n">
         <v>0</v>
@@ -8875,12 +7645,12 @@
       </c>
       <c r="L21" s="67" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>43%</t>
         </is>
       </c>
       <c r="M21" s="67" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>19%</t>
         </is>
       </c>
       <c r="N21" s="67" t="inlineStr">
@@ -9024,10 +7794,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>17</v>
@@ -9046,7 +7816,7 @@
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>58.6%</t>
+          <t>68.4%</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
@@ -9078,10 +7848,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>2</v>
@@ -9100,7 +7870,7 @@
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
-          <t>47.6%</t>
+          <t>59.5%</t>
         </is>
       </c>
       <c r="M4" s="5" t="inlineStr">
@@ -9138,10 +7908,10 @@
         <v>2</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
@@ -9159,7 +7929,7 @@
       </c>
       <c r="M5" s="5" t="inlineStr">
         <is>
-          <t>61.5%</t>
+          <t>69.2%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
@@ -9192,10 +7962,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
@@ -9213,7 +7983,7 @@
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>33.3%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -9290,16 +8060,16 @@
         <v>52</v>
       </c>
       <c r="E8" s="67" t="n">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="F8" s="67" t="n">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="G8" s="67" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H8" s="67" t="n">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I8" s="67" t="n">
         <v>0</v>
@@ -9312,12 +8082,12 @@
       </c>
       <c r="L8" s="67" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="M8" s="67" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="N8" s="67" t="inlineStr">
@@ -9445,10 +8215,10 @@
         <v>2</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
@@ -9466,7 +8236,7 @@
       </c>
       <c r="M12" s="5" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
       <c r="N12" s="5" t="inlineStr">
@@ -9499,13 +8269,13 @@
         <v>2</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>0</v>
@@ -9520,7 +8290,7 @@
       </c>
       <c r="M13" s="5" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>58.3%</t>
         </is>
       </c>
       <c r="N13" s="5" t="inlineStr">
@@ -9544,22 +8314,22 @@
         <v>28</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>0</v>
@@ -9569,12 +8339,12 @@
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>67.9%</t>
         </is>
       </c>
       <c r="M14" s="5" t="inlineStr">
         <is>
-          <t>25.0%</t>
+          <t>32.1%</t>
         </is>
       </c>
       <c r="N14" s="5" t="inlineStr">
@@ -9613,7 +8383,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
@@ -9652,7 +8422,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>7</v>
@@ -9667,7 +8437,7 @@
         <v>7</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>0</v>
@@ -9706,13 +8476,13 @@
         <v>45</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>33</v>
@@ -9721,7 +8491,7 @@
         <v>12</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J17" s="5" t="n">
         <v>0</v>
@@ -9731,7 +8501,7 @@
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
-          <t>82.2%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="M17" s="5" t="inlineStr">
@@ -9812,22 +8582,22 @@
         <v>204</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>0</v>
@@ -9837,12 +8607,12 @@
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
-          <t>44.6%</t>
+          <t>43.6%</t>
         </is>
       </c>
       <c r="M19" s="5" t="inlineStr">
         <is>
-          <t>13.7%</t>
+          <t>15.2%</t>
         </is>
       </c>
       <c r="N19" s="5" t="inlineStr">
@@ -9866,7 +8636,7 @@
         <v>73</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>19</v>
@@ -9875,13 +8645,13 @@
         <v>54</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J20" s="5" t="n">
         <v>0</v>
@@ -9896,7 +8666,7 @@
       </c>
       <c r="M20" s="5" t="inlineStr">
         <is>
-          <t>8.2%</t>
+          <t>15.1%</t>
         </is>
       </c>
       <c r="N20" s="5" t="inlineStr">
@@ -9920,7 +8690,7 @@
         <v>66</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>19</v>
@@ -9929,13 +8699,13 @@
         <v>47</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J21" s="5" t="n">
         <v>0</v>
@@ -9950,7 +8720,7 @@
       </c>
       <c r="M21" s="5" t="inlineStr">
         <is>
-          <t>9.1%</t>
+          <t>19.7%</t>
         </is>
       </c>
       <c r="N21" s="5" t="inlineStr">
@@ -9983,13 +8753,13 @@
         <v>4</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H22" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I22" s="5" t="n">
         <v>7</v>
-      </c>
-      <c r="I22" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="J22" s="5" t="n">
         <v>0</v>
@@ -10004,7 +8774,7 @@
       </c>
       <c r="M22" s="5" t="inlineStr">
         <is>
-          <t>65.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="N22" s="5" t="inlineStr">
@@ -10028,13 +8798,13 @@
         <v>11</v>
       </c>
       <c r="D23" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E23" s="5" t="n">
-        <v>4</v>
-      </c>
       <c r="F23" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>2</v>
@@ -10043,7 +8813,7 @@
         <v>9</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="5" t="n">
         <v>0</v>
@@ -10053,7 +8823,7 @@
       </c>
       <c r="L23" s="5" t="inlineStr">
         <is>
-          <t>36.4%</t>
+          <t>27.3%</t>
         </is>
       </c>
       <c r="M23" s="5" t="inlineStr">
@@ -10136,7 +8906,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>0</v>
@@ -10240,22 +9010,22 @@
         <v>506</v>
       </c>
       <c r="D27" s="67" t="n">
-        <v>178</v>
+        <v>263</v>
       </c>
       <c r="E27" s="67" t="n">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F27" s="67" t="n">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="G27" s="67" t="n">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="H27" s="67" t="n">
-        <v>398</v>
+        <v>373</v>
       </c>
       <c r="I27" s="67" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="J27" s="67" t="n">
         <v>0</v>
@@ -10265,12 +9035,12 @@
       </c>
       <c r="L27" s="67" t="inlineStr">
         <is>
-          <t>46%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="M27" s="67" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="N27" s="67" t="inlineStr">
@@ -10404,7 +9174,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J31" s="5" t="n">
         <v>0</v>
@@ -10452,13 +9222,13 @@
         <v>2</v>
       </c>
       <c r="G32" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>0</v>
@@ -10473,7 +9243,7 @@
       </c>
       <c r="M32" s="5" t="inlineStr">
         <is>
-          <t>70.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
       <c r="N32" s="5" t="inlineStr">
@@ -10556,13 +9326,13 @@
         <v>8</v>
       </c>
       <c r="G34" s="67" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H34" s="67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I34" s="67" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J34" s="67" t="n">
         <v>0</v>
@@ -10577,7 +9347,7 @@
       </c>
       <c r="M34" s="67" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="N34" s="67" t="inlineStr">
@@ -11060,10 +9830,10 @@
         <v>0</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G46" s="5" t="n">
         <v>0</v>
@@ -11082,7 +9852,7 @@
       </c>
       <c r="L46" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="M46" s="5" t="inlineStr">
@@ -11114,10 +9884,10 @@
         <v>0</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F47" s="5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G47" s="5" t="n">
         <v>0</v>
@@ -11136,7 +9906,7 @@
       </c>
       <c r="L47" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>90.0%</t>
         </is>
       </c>
       <c r="M47" s="5" t="inlineStr">
@@ -11164,10 +9934,10 @@
         <v>0</v>
       </c>
       <c r="E48" s="67" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F48" s="67" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G48" s="67" t="n">
         <v>0</v>
@@ -11186,7 +9956,7 @@
       </c>
       <c r="L48" s="67" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="M48" s="67" t="inlineStr">
@@ -11690,7 +10460,7 @@
         </is>
       </c>
       <c r="B1" s="26" t="n">
-        <v>307</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2">
@@ -11700,7 +10470,7 @@
         </is>
       </c>
       <c r="B2" s="26" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
@@ -11710,7 +10480,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>203</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4">
@@ -11720,7 +10490,7 @@
         </is>
       </c>
       <c r="B4" s="26" t="n">
-        <v>54</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
@@ -11730,7 +10500,7 @@
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>103</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6">
@@ -11740,7 +10510,7 @@
         </is>
       </c>
       <c r="B6" s="26" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -11770,7 +10540,7 @@
         </is>
       </c>
       <c r="B9" s="26" t="n">
-        <v>294</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -11806,7 +10576,7 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>412 Workable</t>
+          <t>437 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -11881,7 +10651,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>456</v>
+        <v>347</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11901,7 +10671,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11973,7 +10743,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>3198.2</v>
+        <v>3310.2</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -12061,7 +10831,7 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>412 Workable</t>
+          <t>437 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -12136,7 +10906,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>423</v>
+        <v>337</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -12156,7 +10926,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -12176,7 +10946,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -12228,7 +10998,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>1245</v>
+        <v>1357</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -12292,7 +11062,7 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>412 Workable</t>
+          <t>437 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -12367,7 +11137,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -12387,7 +11157,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -12407,7 +11177,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -12564,7 +11334,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
@@ -12610,7 +11380,7 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>412 Workable</t>
+          <t>437 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -12725,7 +11495,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -12751,7 +11521,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -12777,7 +11547,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>0</v>
@@ -12825,7 +11595,7 @@
       <c r="C10" s="5" t="n"/>
       <c r="D10" s="5" t="n"/>
       <c r="E10" s="22" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F10" s="5" t="n"/>
       <c r="G10" s="5" t="n"/>
@@ -12863,7 +11633,7 @@
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="22" t="n">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F12" s="5" t="n"/>
       <c r="G12" s="5" t="n"/>

</xml_diff>

<commit_message>
Add load number to spool object
</commit_message>
<xml_diff>
--- a/database/7052/JobSummary.xlsx
+++ b/database/7052/JobSummary.xlsx
@@ -4478,27 +4478,23 @@
       <c r="B1" s="51" t="n"/>
       <c r="C1" s="52" t="inlineStr">
         <is>
-          <t>1194  Spools</t>
+          <t>1188  Spools</t>
         </is>
       </c>
       <c r="D1" s="53" t="n"/>
       <c r="E1" s="54" t="inlineStr">
         <is>
-          <t>1045  Workable</t>
+          <t>1081  Workable</t>
         </is>
       </c>
       <c r="F1" s="55" t="n"/>
       <c r="G1" s="52" t="inlineStr">
         <is>
-          <t>965  Issued</t>
+          <t>1081  Issued</t>
         </is>
       </c>
       <c r="H1" s="56" t="n"/>
-      <c r="I1" s="57" t="inlineStr">
-        <is>
-          <t>6335  Workable Man Hours</t>
-        </is>
-      </c>
+      <c r="I1" s="57" t="n"/>
       <c r="J1" s="58" t="n"/>
       <c r="K1" s="58" t="n"/>
     </row>
@@ -4601,15 +4597,9 @@
         </is>
       </c>
       <c r="H5" s="70" t="n"/>
-      <c r="I5" s="43" t="n">
-        <v>453</v>
-      </c>
-      <c r="J5" s="43" t="n">
-        <v>5882</v>
-      </c>
-      <c r="K5" s="44" t="n">
-        <v>6335</v>
-      </c>
+      <c r="I5" s="43" t="n"/>
+      <c r="J5" s="43" t="n"/>
+      <c r="K5" s="44" t="n"/>
     </row>
     <row r="6" ht="18.75" customFormat="1" customHeight="1" s="1">
       <c r="A6" s="46" t="inlineStr">
@@ -5604,10 +5594,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>3</v>
@@ -5626,7 +5616,7 @@
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="M35" s="1" t="inlineStr">
@@ -5658,39 +5648,39 @@
         <v>2</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="1" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t>94.3%</t>
+          <t>98.4%</t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>52.8%</t>
+          <t>62.6%</t>
         </is>
       </c>
       <c r="N36" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>41.5%</t>
         </is>
       </c>
     </row>
@@ -5712,10 +5702,10 @@
         <v>0</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>43</v>
@@ -5724,7 +5714,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J37" s="1" t="n">
         <v>0</v>
@@ -5734,7 +5724,7 @@
       </c>
       <c r="L37" s="1" t="inlineStr">
         <is>
-          <t>95.6%</t>
+          <t>97.8%</t>
         </is>
       </c>
       <c r="M37" s="1" t="inlineStr">
@@ -5763,42 +5753,42 @@
         <v>255</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="J38" s="1" t="n">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="L38" s="1" t="inlineStr">
         <is>
-          <t>80.8%</t>
+          <t>90.2%</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
         <is>
-          <t>70.2%</t>
+          <t>78.4%</t>
         </is>
       </c>
       <c r="N38" s="1" t="inlineStr">
         <is>
-          <t>14.1%</t>
+          <t>24.7%</t>
         </is>
       </c>
     </row>
@@ -5814,45 +5804,45 @@
         </is>
       </c>
       <c r="C39" s="1" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D39" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="F39" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="E39" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="F39" s="1" t="n">
-        <v>18</v>
-      </c>
       <c r="G39" s="1" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="J39" s="1" t="n">
         <v>22</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L39" s="1" t="inlineStr">
         <is>
-          <t>79.8%</t>
+          <t>83.7%</t>
         </is>
       </c>
       <c r="M39" s="1" t="inlineStr">
         <is>
-          <t>74.2%</t>
+          <t>80.2%</t>
         </is>
       </c>
       <c r="N39" s="1" t="inlineStr">
         <is>
-          <t>24.7%</t>
+          <t>25.6%</t>
         </is>
       </c>
     </row>
@@ -5868,45 +5858,45 @@
         </is>
       </c>
       <c r="C40" s="1" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>19</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>66</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="J40" s="1" t="n">
         <v>19</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L40" s="1" t="inlineStr">
         <is>
-          <t>75.3%</t>
+          <t>75.6%</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>71.0%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="N40" s="1" t="inlineStr">
         <is>
-          <t>20.4%</t>
+          <t>21.1%</t>
         </is>
       </c>
     </row>
@@ -5928,10 +5918,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>40</v>
@@ -5943,24 +5933,24 @@
         <v>28</v>
       </c>
       <c r="J41" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L41" s="1" t="inlineStr">
         <is>
+          <t>97.6%</t>
+        </is>
+      </c>
+      <c r="M41" s="1" t="inlineStr">
+        <is>
           <t>95.2%</t>
         </is>
       </c>
-      <c r="M41" s="1" t="inlineStr">
-        <is>
-          <t>95.2%</t>
-        </is>
-      </c>
       <c r="N41" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>19.0%</t>
         </is>
       </c>
     </row>
@@ -5988,10 +5978,10 @@
         <v>1</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>11</v>
@@ -6009,7 +5999,7 @@
       </c>
       <c r="M42" s="1" t="inlineStr">
         <is>
-          <t>95.2%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N42" s="1" t="inlineStr">
@@ -6033,42 +6023,42 @@
         <v>158</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="G43" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="H43" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G43" s="1" t="n">
-        <v>136</v>
-      </c>
-      <c r="H43" s="1" t="n">
-        <v>22</v>
-      </c>
       <c r="I43" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="1" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="L43" s="1" t="inlineStr">
         <is>
+          <t>93.0%</t>
+        </is>
+      </c>
+      <c r="M43" s="1" t="inlineStr">
+        <is>
           <t>90.5%</t>
         </is>
       </c>
-      <c r="M43" s="1" t="inlineStr">
-        <is>
-          <t>86.1%</t>
-        </is>
-      </c>
       <c r="N43" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>54.4%</t>
         </is>
       </c>
     </row>
@@ -6105,10 +6095,10 @@
         <v>0</v>
       </c>
       <c r="J44" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K44" s="1" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L44" s="1" t="inlineStr">
         <is>
@@ -6122,7 +6112,7 @@
       </c>
       <c r="N44" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>4.8%</t>
         </is>
       </c>
     </row>
@@ -6159,10 +6149,10 @@
         <v>1</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K45" s="1" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="L45" s="1" t="inlineStr">
         <is>
@@ -6176,7 +6166,7 @@
       </c>
       <c r="N45" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>23.1%</t>
         </is>
       </c>
     </row>
@@ -6195,19 +6185,19 @@
         <v>10</v>
       </c>
       <c r="D46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F46" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="G46" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F46" s="1" t="n">
+      <c r="H46" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="G46" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H46" s="1" t="n">
-        <v>6</v>
       </c>
       <c r="I46" s="1" t="n">
         <v>1</v>
@@ -6220,12 +6210,12 @@
       </c>
       <c r="L46" s="1" t="inlineStr">
         <is>
+          <t>70.0%</t>
+        </is>
+      </c>
+      <c r="M46" s="1" t="inlineStr">
+        <is>
           <t>50.0%</t>
-        </is>
-      </c>
-      <c r="M46" s="1" t="inlineStr">
-        <is>
-          <t>40.0%</t>
         </is>
       </c>
       <c r="N46" s="1" t="inlineStr">
@@ -6267,10 +6257,10 @@
         <v>0</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L47" s="1" t="inlineStr">
         <is>
@@ -6284,7 +6274,7 @@
       </c>
       <c r="N47" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>33.3%</t>
         </is>
       </c>
     </row>
@@ -6312,10 +6302,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>8</v>
@@ -6333,7 +6323,7 @@
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>88.9%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N48" s="1" t="inlineStr">
@@ -6366,19 +6356,19 @@
         <v>0</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J49" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K49" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L49" s="1" t="inlineStr">
         <is>
@@ -6387,12 +6377,12 @@
       </c>
       <c r="M49" s="1" t="inlineStr">
         <is>
-          <t>90.9%</t>
+          <t>95.5%</t>
         </is>
       </c>
       <c r="N49" s="1" t="inlineStr">
         <is>
-          <t>4.5%</t>
+          <t>13.6%</t>
         </is>
       </c>
     </row>
@@ -6426,13 +6416,13 @@
         <v>0</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J50" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K50" s="1" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L50" s="1" t="inlineStr">
         <is>
@@ -6446,7 +6436,7 @@
       </c>
       <c r="N50" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>12.0%</t>
         </is>
       </c>
     </row>
@@ -6468,10 +6458,10 @@
         <v>6</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G51" s="1" t="n">
         <v>41</v>
@@ -6480,27 +6470,27 @@
         <v>12</v>
       </c>
       <c r="I51" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J51" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K51" s="1" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L51" s="1" t="inlineStr">
         <is>
+          <t>88.7%</t>
+        </is>
+      </c>
+      <c r="M51" s="1" t="inlineStr">
+        <is>
           <t>77.4%</t>
         </is>
       </c>
-      <c r="M51" s="1" t="inlineStr">
-        <is>
-          <t>77.4%</t>
-        </is>
-      </c>
       <c r="N51" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>15.1%</t>
         </is>
       </c>
     </row>
@@ -6564,45 +6554,45 @@
       </c>
       <c r="B53" s="76" t="n"/>
       <c r="C53" s="76" t="n">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="D53" s="76" t="n">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="E53" s="76" t="n">
-        <v>1126</v>
+        <v>1082</v>
       </c>
       <c r="F53" s="76" t="n">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="G53" s="76" t="n">
-        <v>776</v>
+        <v>823</v>
       </c>
       <c r="H53" s="76" t="n">
-        <v>418</v>
+        <v>365</v>
       </c>
       <c r="I53" s="76" t="n">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="J53" s="76" t="n">
-        <v>78</v>
+        <v>275</v>
       </c>
       <c r="K53" s="76" t="n">
-        <v>1116</v>
+        <v>913</v>
       </c>
       <c r="L53" s="76" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="M53" s="76" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="N53" s="76" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>23%</t>
         </is>
       </c>
     </row>
@@ -6850,10 +6840,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>3</v>
@@ -6872,7 +6862,7 @@
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="M4" s="5" t="inlineStr">
@@ -6904,39 +6894,39 @@
         <v>2</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>94.3%</t>
+          <t>98.4%</t>
         </is>
       </c>
       <c r="M5" s="5" t="inlineStr">
         <is>
-          <t>52.8%</t>
+          <t>62.6%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>41.5%</t>
         </is>
       </c>
     </row>
@@ -6958,10 +6948,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>43</v>
@@ -6970,7 +6960,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
@@ -6980,7 +6970,7 @@
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>95.6%</t>
+          <t>97.8%</t>
         </is>
       </c>
       <c r="M6" s="5" t="inlineStr">
@@ -7009,42 +6999,42 @@
         <v>255</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>80.8%</t>
+          <t>90.2%</t>
         </is>
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>70.2%</t>
+          <t>78.4%</t>
         </is>
       </c>
       <c r="N7" s="5" t="inlineStr">
         <is>
-          <t>14.1%</t>
+          <t>24.7%</t>
         </is>
       </c>
     </row>
@@ -7060,45 +7050,45 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D8" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>72</v>
+      </c>
+      <c r="F8" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E8" s="5" t="n">
-        <v>71</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>18</v>
-      </c>
       <c r="G8" s="5" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>22</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>79.8%</t>
+          <t>83.7%</t>
         </is>
       </c>
       <c r="M8" s="5" t="inlineStr">
         <is>
-          <t>74.2%</t>
+          <t>80.2%</t>
         </is>
       </c>
       <c r="N8" s="5" t="inlineStr">
         <is>
-          <t>24.7%</t>
+          <t>25.6%</t>
         </is>
       </c>
     </row>
@@ -7114,45 +7104,45 @@
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>19</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>66</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="J9" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>75.3%</t>
+          <t>75.6%</t>
         </is>
       </c>
       <c r="M9" s="5" t="inlineStr">
         <is>
-          <t>71.0%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="N9" s="5" t="inlineStr">
         <is>
-          <t>20.4%</t>
+          <t>21.1%</t>
         </is>
       </c>
     </row>
@@ -7174,10 +7164,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>40</v>
@@ -7189,24 +7179,24 @@
         <v>28</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
+          <t>97.6%</t>
+        </is>
+      </c>
+      <c r="M10" s="5" t="inlineStr">
+        <is>
           <t>95.2%</t>
         </is>
       </c>
-      <c r="M10" s="5" t="inlineStr">
-        <is>
-          <t>95.2%</t>
-        </is>
-      </c>
       <c r="N10" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>19.0%</t>
         </is>
       </c>
     </row>
@@ -7234,10 +7224,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5" t="n">
         <v>11</v>
@@ -7255,7 +7245,7 @@
       </c>
       <c r="M11" s="5" t="inlineStr">
         <is>
-          <t>95.2%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N11" s="5" t="inlineStr">
@@ -7279,42 +7269,42 @@
         <v>158</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E12" s="5" t="n">
+        <v>147</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5" t="n">
         <v>143</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="H12" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G12" s="5" t="n">
-        <v>136</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <v>22</v>
-      </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
+          <t>93.0%</t>
+        </is>
+      </c>
+      <c r="M12" s="5" t="inlineStr">
+        <is>
           <t>90.5%</t>
         </is>
       </c>
-      <c r="M12" s="5" t="inlineStr">
-        <is>
-          <t>86.1%</t>
-        </is>
-      </c>
       <c r="N12" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>54.4%</t>
         </is>
       </c>
     </row>
@@ -7351,10 +7341,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L13" s="5" t="inlineStr">
         <is>
@@ -7368,7 +7358,7 @@
       </c>
       <c r="N13" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>4.8%</t>
         </is>
       </c>
     </row>
@@ -7405,10 +7395,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
@@ -7422,7 +7412,7 @@
       </c>
       <c r="N14" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>23.1%</t>
         </is>
       </c>
     </row>
@@ -7441,19 +7431,19 @@
         <v>10</v>
       </c>
       <c r="D15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="G15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="H15" s="5" t="n">
         <v>5</v>
-      </c>
-      <c r="G15" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H15" s="5" t="n">
-        <v>6</v>
       </c>
       <c r="I15" s="5" t="n">
         <v>1</v>
@@ -7466,12 +7456,12 @@
       </c>
       <c r="L15" s="5" t="inlineStr">
         <is>
+          <t>70.0%</t>
+        </is>
+      </c>
+      <c r="M15" s="5" t="inlineStr">
+        <is>
           <t>50.0%</t>
-        </is>
-      </c>
-      <c r="M15" s="5" t="inlineStr">
-        <is>
-          <t>40.0%</t>
         </is>
       </c>
       <c r="N15" s="5" t="inlineStr">
@@ -7513,10 +7503,10 @@
         <v>0</v>
       </c>
       <c r="J16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L16" s="5" t="inlineStr">
         <is>
@@ -7530,7 +7520,7 @@
       </c>
       <c r="N16" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>33.3%</t>
         </is>
       </c>
     </row>
@@ -7558,10 +7548,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>8</v>
@@ -7579,7 +7569,7 @@
       </c>
       <c r="M17" s="5" t="inlineStr">
         <is>
-          <t>88.9%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -7612,19 +7602,19 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
@@ -7633,12 +7623,12 @@
       </c>
       <c r="M18" s="5" t="inlineStr">
         <is>
-          <t>90.9%</t>
+          <t>95.5%</t>
         </is>
       </c>
       <c r="N18" s="5" t="inlineStr">
         <is>
-          <t>4.5%</t>
+          <t>13.6%</t>
         </is>
       </c>
     </row>
@@ -7672,13 +7662,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
@@ -7692,7 +7682,7 @@
       </c>
       <c r="N19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>12.0%</t>
         </is>
       </c>
     </row>
@@ -7714,10 +7704,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>41</v>
@@ -7726,27 +7716,27 @@
         <v>12</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L20" s="5" t="inlineStr">
         <is>
+          <t>88.7%</t>
+        </is>
+      </c>
+      <c r="M20" s="5" t="inlineStr">
+        <is>
           <t>77.4%</t>
         </is>
       </c>
-      <c r="M20" s="5" t="inlineStr">
-        <is>
-          <t>77.4%</t>
-        </is>
-      </c>
       <c r="N20" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>15.1%</t>
         </is>
       </c>
     </row>
@@ -7810,45 +7800,45 @@
       </c>
       <c r="B22" s="79" t="n"/>
       <c r="C22" s="79" t="n">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="D22" s="79" t="n">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="E22" s="79" t="n">
-        <v>1045</v>
+        <v>1081</v>
       </c>
       <c r="F22" s="79" t="n">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="G22" s="79" t="n">
-        <v>776</v>
+        <v>823</v>
       </c>
       <c r="H22" s="79" t="n">
-        <v>418</v>
+        <v>365</v>
       </c>
       <c r="I22" s="79" t="n">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="J22" s="79" t="n">
-        <v>78</v>
+        <v>275</v>
       </c>
       <c r="K22" s="79" t="n">
-        <v>1116</v>
+        <v>913</v>
       </c>
       <c r="L22" s="79" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="M22" s="79" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="N22" s="79" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>23%</t>
         </is>
       </c>
     </row>
@@ -7866,7 +7856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
@@ -7993,19 +7983,19 @@
         <v>11</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>154</v>
+        <v>68</v>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
@@ -8014,12 +8004,12 @@
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>88.3%</t>
+          <t>92.2%</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>55.8%</t>
         </is>
       </c>
     </row>
@@ -8056,10 +8046,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
@@ -8073,7 +8063,7 @@
       </c>
       <c r="N4" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>4.8%</t>
         </is>
       </c>
     </row>
@@ -8110,10 +8100,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
@@ -8127,7 +8117,7 @@
       </c>
       <c r="N5" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>23.1%</t>
         </is>
       </c>
     </row>
@@ -8155,20 +8145,20 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>12</v>
-      </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
           <t>100%</t>
@@ -8176,12 +8166,12 @@
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>83.3%</t>
+          <t>91.7%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>16.7%</t>
         </is>
       </c>
     </row>
@@ -8200,13 +8190,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>33</v>
@@ -8218,24 +8208,24 @@
         <v>0</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M7" s="5" t="inlineStr">
+        <is>
           <t>86.8%</t>
         </is>
       </c>
-      <c r="M7" s="5" t="inlineStr">
-        <is>
-          <t>86.8%</t>
-        </is>
-      </c>
       <c r="N7" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>71.1%</t>
         </is>
       </c>
     </row>
@@ -8300,42 +8290,42 @@
         <v>290</v>
       </c>
       <c r="D9" s="79" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E9" s="79" t="n">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="F9" s="79" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G9" s="79" t="n">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="H9" s="79" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I9" s="79" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="79" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K9" s="79" t="n">
-        <v>290</v>
+        <v>170</v>
       </c>
       <c r="L9" s="79" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="M9" s="79" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="N9" s="79" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>41%</t>
         </is>
       </c>
     </row>
@@ -8464,7 +8454,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>1</v>
@@ -8518,7 +8508,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>0</v>
@@ -8572,7 +8562,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
@@ -8674,10 +8664,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>8</v>
@@ -8695,7 +8685,7 @@
       </c>
       <c r="M17" s="5" t="inlineStr">
         <is>
-          <t>88.9%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N17" s="5" t="inlineStr">
@@ -8722,10 +8712,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="5" t="n">
         <v>43</v>
@@ -8734,7 +8724,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J18" s="5" t="n">
         <v>0</v>
@@ -8744,7 +8734,7 @@
       </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
-          <t>95.6%</t>
+          <t>97.8%</t>
         </is>
       </c>
       <c r="M18" s="5" t="inlineStr">
@@ -8825,22 +8815,22 @@
         <v>217</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="J20" s="5" t="n">
         <v>36</v>
@@ -8850,12 +8840,12 @@
       </c>
       <c r="L20" s="5" t="inlineStr">
         <is>
-          <t>79.7%</t>
+          <t>88.5%</t>
         </is>
       </c>
       <c r="M20" s="5" t="inlineStr">
         <is>
-          <t>67.3%</t>
+          <t>77.0%</t>
         </is>
       </c>
       <c r="N20" s="5" t="inlineStr">
@@ -8882,10 +8872,10 @@
         <v>19</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="5" t="n">
         <v>40</v>
@@ -8894,7 +8884,7 @@
         <v>21</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J21" s="5" t="n">
         <v>2</v>
@@ -8904,7 +8894,7 @@
       </c>
       <c r="L21" s="5" t="inlineStr">
         <is>
-          <t>67.2%</t>
+          <t>68.9%</t>
         </is>
       </c>
       <c r="M21" s="5" t="inlineStr">
@@ -8933,22 +8923,22 @@
         <v>57</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J22" s="5" t="n">
         <v>1</v>
@@ -8958,12 +8948,12 @@
       </c>
       <c r="L22" s="5" t="inlineStr">
         <is>
-          <t>77.2%</t>
+          <t>80.7%</t>
         </is>
       </c>
       <c r="M22" s="5" t="inlineStr">
         <is>
-          <t>73.7%</t>
+          <t>75.4%</t>
         </is>
       </c>
       <c r="N22" s="5" t="inlineStr">
@@ -9050,10 +9040,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="5" t="n">
         <v>4</v>
@@ -9071,7 +9061,7 @@
       </c>
       <c r="M24" s="5" t="inlineStr">
         <is>
-          <t>90.9%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N24" s="5" t="inlineStr">
@@ -9095,19 +9085,19 @@
         <v>4</v>
       </c>
       <c r="D25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E25" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="F25" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I25" s="5" t="n">
         <v>0</v>
@@ -9120,12 +9110,12 @@
       </c>
       <c r="L25" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="M25" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>25.0%</t>
         </is>
       </c>
       <c r="N25" s="5" t="inlineStr">
@@ -9149,19 +9139,19 @@
         <v>10</v>
       </c>
       <c r="D26" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F26" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="G26" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="H26" s="5" t="n">
         <v>5</v>
-      </c>
-      <c r="G26" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H26" s="5" t="n">
-        <v>6</v>
       </c>
       <c r="I26" s="5" t="n">
         <v>1</v>
@@ -9174,12 +9164,12 @@
       </c>
       <c r="L26" s="5" t="inlineStr">
         <is>
+          <t>70.0%</t>
+        </is>
+      </c>
+      <c r="M26" s="5" t="inlineStr">
+        <is>
           <t>50.0%</t>
-        </is>
-      </c>
-      <c r="M26" s="5" t="inlineStr">
-        <is>
-          <t>40.0%</t>
         </is>
       </c>
       <c r="N26" s="5" t="inlineStr">
@@ -9253,22 +9243,22 @@
         <v>494</v>
       </c>
       <c r="D28" s="79" t="n">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="E28" s="79" t="n">
-        <v>403</v>
+        <v>432</v>
       </c>
       <c r="F28" s="79" t="n">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="G28" s="79" t="n">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="H28" s="79" t="n">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="I28" s="79" t="n">
-        <v>237</v>
+        <v>275</v>
       </c>
       <c r="J28" s="79" t="n">
         <v>40</v>
@@ -9278,12 +9268,12 @@
       </c>
       <c r="L28" s="79" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="M28" s="79" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="N28" s="79" t="inlineStr">
@@ -9712,39 +9702,39 @@
         <v>2</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F39" s="5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G39" s="5" t="n">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J39" s="5" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="L39" s="5" t="inlineStr">
         <is>
-          <t>94.3%</t>
+          <t>98.4%</t>
         </is>
       </c>
       <c r="M39" s="5" t="inlineStr">
         <is>
-          <t>53.3%</t>
+          <t>63.1%</t>
         </is>
       </c>
       <c r="N39" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>41.8%</t>
         </is>
       </c>
     </row>
@@ -9766,10 +9756,10 @@
         <v>6</v>
       </c>
       <c r="E40" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="F40" s="5" t="n">
         <v>6</v>
-      </c>
-      <c r="F40" s="5" t="n">
-        <v>11</v>
       </c>
       <c r="G40" s="5" t="n">
         <v>6</v>
@@ -9781,24 +9771,24 @@
         <v>0</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K40" s="5" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L40" s="5" t="inlineStr">
         <is>
+          <t>64.7%</t>
+        </is>
+      </c>
+      <c r="M40" s="5" t="inlineStr">
+        <is>
           <t>35.3%</t>
         </is>
       </c>
-      <c r="M40" s="5" t="inlineStr">
+      <c r="N40" s="5" t="inlineStr">
         <is>
           <t>35.3%</t>
-        </is>
-      </c>
-      <c r="N40" s="5" t="inlineStr">
-        <is>
-          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -9835,10 +9825,10 @@
         <v>0</v>
       </c>
       <c r="J41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L41" s="5" t="inlineStr">
         <is>
@@ -9852,7 +9842,7 @@
       </c>
       <c r="N41" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>33.3%</t>
         </is>
       </c>
     </row>
@@ -9889,10 +9879,10 @@
         <v>0</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K42" s="5" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="L42" s="5" t="inlineStr">
         <is>
@@ -9906,7 +9896,7 @@
       </c>
       <c r="N42" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>25.7%</t>
         </is>
       </c>
     </row>
@@ -9974,39 +9964,39 @@
         <v>21</v>
       </c>
       <c r="E44" s="79" t="n">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="F44" s="79" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G44" s="79" t="n">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="H44" s="79" t="n">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="I44" s="79" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="79" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K44" s="79" t="n">
-        <v>299</v>
+        <v>232</v>
       </c>
       <c r="L44" s="79" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="M44" s="79" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>32%</t>
         </is>
       </c>
       <c r="N44" s="79" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>22%</t>
         </is>
       </c>
     </row>
@@ -10123,10 +10113,10 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F48" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>3</v>
@@ -10138,24 +10128,24 @@
         <v>0</v>
       </c>
       <c r="J48" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K48" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L48" s="5" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M48" s="5" t="inlineStr">
+        <is>
           <t>75.0%</t>
         </is>
       </c>
-      <c r="M48" s="5" t="inlineStr">
-        <is>
-          <t>75.0%</t>
-        </is>
-      </c>
       <c r="N48" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -10177,10 +10167,10 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F49" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>9</v>
@@ -10192,24 +10182,24 @@
         <v>0</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K49" s="5" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L49" s="5" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M49" s="5" t="inlineStr">
+        <is>
           <t>90.0%</t>
         </is>
       </c>
-      <c r="M49" s="5" t="inlineStr">
-        <is>
-          <t>90.0%</t>
-        </is>
-      </c>
       <c r="N49" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
     </row>
@@ -10227,10 +10217,10 @@
         <v>0</v>
       </c>
       <c r="E50" s="79" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F50" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G50" s="79" t="n">
         <v>12</v>
@@ -10242,24 +10232,24 @@
         <v>0</v>
       </c>
       <c r="J50" s="79" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K50" s="79" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="L50" s="79" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M50" s="79" t="inlineStr">
+        <is>
           <t>86%</t>
         </is>
       </c>
-      <c r="M50" s="79" t="inlineStr">
-        <is>
-          <t>86%</t>
-        </is>
-      </c>
       <c r="N50" s="79" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>71%</t>
         </is>
       </c>
     </row>
@@ -10370,45 +10360,45 @@
         </is>
       </c>
       <c r="C54" s="5" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D54" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F54" s="5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G54" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H54" s="5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I54" s="5" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J54" s="5" t="n">
         <v>21</v>
       </c>
       <c r="K54" s="5" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L54" s="5" t="inlineStr">
         <is>
-          <t>84.4%</t>
+          <t>89.7%</t>
         </is>
       </c>
       <c r="M54" s="5" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>89.7%</t>
         </is>
       </c>
       <c r="N54" s="5" t="inlineStr">
         <is>
-          <t>65.6%</t>
+          <t>72.4%</t>
         </is>
       </c>
     </row>
@@ -10424,13 +10414,13 @@
         </is>
       </c>
       <c r="C55" s="5" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F55" s="5" t="n">
         <v>3</v>
@@ -10439,30 +10429,30 @@
         <v>26</v>
       </c>
       <c r="H55" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I55" s="5" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>17</v>
       </c>
       <c r="K55" s="5" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L55" s="5" t="inlineStr">
         <is>
-          <t>90.6%</t>
+          <t>89.7%</t>
         </is>
       </c>
       <c r="M55" s="5" t="inlineStr">
         <is>
-          <t>81.3%</t>
+          <t>89.7%</t>
         </is>
       </c>
       <c r="N55" s="5" t="inlineStr">
         <is>
-          <t>53.1%</t>
+          <t>58.6%</t>
         </is>
       </c>
     </row>
@@ -10474,45 +10464,45 @@
       </c>
       <c r="B56" s="79" t="n"/>
       <c r="C56" s="79" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D56" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E56" s="79" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F56" s="79" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G56" s="79" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H56" s="79" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I56" s="79" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J56" s="79" t="n">
         <v>38</v>
       </c>
       <c r="K56" s="79" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L56" s="79" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="M56" s="79" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="N56" s="79" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>66%</t>
         </is>
       </c>
     </row>
@@ -10535,7 +10525,7 @@
     <row r="58" ht="37" customHeight="1">
       <c r="A58" s="77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Summary</t>
+          <t>A105 Summary</t>
         </is>
       </c>
     </row>
@@ -10666,111 +10656,256 @@
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
-      <c r="A61" s="5" t="inlineStr">
+      <c r="A61" s="79" t="inlineStr">
+        <is>
+          <t>TOTALS</t>
+        </is>
+      </c>
+      <c r="B61" s="79" t="n"/>
+      <c r="C61" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="I61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L61" s="79" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M61" s="79" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="N61" s="79" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="15" customHeight="1">
+      <c r="A62" s="5" t="n"/>
+      <c r="B62" s="5" t="n"/>
+      <c r="C62" s="5" t="n"/>
+      <c r="D62" s="5" t="n"/>
+      <c r="E62" s="5" t="n"/>
+      <c r="F62" s="5" t="n"/>
+      <c r="G62" s="5" t="n"/>
+      <c r="H62" s="5" t="n"/>
+      <c r="I62" s="5" t="n"/>
+      <c r="J62" s="5" t="n"/>
+      <c r="K62" s="5" t="n"/>
+      <c r="L62" s="5" t="n"/>
+      <c r="M62" s="5" t="n"/>
+      <c r="N62" s="5" t="n"/>
+    </row>
+    <row r="63" ht="37" customHeight="1">
+      <c r="A63" s="77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="37" customHeight="1">
+      <c r="A64" s="78" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="B64" s="78" t="inlineStr">
+        <is>
+          <t>Priority #</t>
+        </is>
+      </c>
+      <c r="C64" s="78" t="inlineStr">
+        <is>
+          <t>Total Spools</t>
+        </is>
+      </c>
+      <c r="D64" s="78" t="inlineStr">
+        <is>
+          <t>On Hold</t>
+        </is>
+      </c>
+      <c r="E64" s="78" t="inlineStr">
+        <is>
+          <t>Workable</t>
+        </is>
+      </c>
+      <c r="F64" s="78" t="inlineStr">
+        <is>
+          <t>Not Workable</t>
+        </is>
+      </c>
+      <c r="G64" s="78" t="inlineStr">
+        <is>
+          <t>Welded Out</t>
+        </is>
+      </c>
+      <c r="H64" s="78" t="inlineStr">
+        <is>
+          <t>Remaining to Weld Out</t>
+        </is>
+      </c>
+      <c r="I64" s="78" t="inlineStr">
+        <is>
+          <t>Shipped To Paint</t>
+        </is>
+      </c>
+      <c r="J64" s="78" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="K64" s="78" t="inlineStr">
+        <is>
+          <t>Remaining to Deliver</t>
+        </is>
+      </c>
+      <c r="L64" s="78" t="inlineStr">
+        <is>
+          <t>Workable %</t>
+        </is>
+      </c>
+      <c r="M64" s="78" t="inlineStr">
+        <is>
+          <t>Weld Out %</t>
+        </is>
+      </c>
+      <c r="N64" s="78" t="inlineStr">
+        <is>
+          <t>Delivered %</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="15" customHeight="1">
+      <c r="A65" s="5" t="inlineStr">
         <is>
           <t>J30</t>
         </is>
       </c>
-      <c r="B61" s="5" t="inlineStr">
+      <c r="B65" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C61" s="5" t="n">
+      <c r="C65" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" s="5" t="n">
+      <c r="D65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="F61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="5" t="n">
+      <c r="G65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="5" t="n">
+      <c r="I65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="L61" s="5" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M61" s="5" t="inlineStr">
+      <c r="L65" s="5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="M65" s="5" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
       </c>
-      <c r="N61" s="5" t="inlineStr">
+      <c r="N65" s="5" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="15" customHeight="1">
-      <c r="A62" s="79" t="inlineStr">
+    <row r="66" ht="15" customHeight="1">
+      <c r="A66" s="79" t="inlineStr">
         <is>
           <t>TOTALS</t>
         </is>
       </c>
-      <c r="B62" s="79" t="n"/>
-      <c r="C62" s="79" t="n">
-        <v>7</v>
-      </c>
-      <c r="D62" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" s="79" t="n">
-        <v>7</v>
-      </c>
-      <c r="F62" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H62" s="79" t="n">
-        <v>7</v>
-      </c>
-      <c r="I62" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="K62" s="79" t="n">
-        <v>7</v>
-      </c>
-      <c r="L62" s="79" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M62" s="79" t="inlineStr">
+      <c r="B66" s="79" t="n"/>
+      <c r="C66" s="79" t="n">
+        <v>6</v>
+      </c>
+      <c r="D66" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="79" t="n">
+        <v>6</v>
+      </c>
+      <c r="G66" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="79" t="n">
+        <v>6</v>
+      </c>
+      <c r="I66" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="79" t="n">
+        <v>6</v>
+      </c>
+      <c r="L66" s="79" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="N62" s="79" t="inlineStr">
+      <c r="M66" s="79" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
+      <c r="N66" s="79" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A11:N11"/>
     <mergeCell ref="A30:N30"/>
@@ -10778,6 +10913,7 @@
     <mergeCell ref="A46:N46"/>
     <mergeCell ref="A52:N52"/>
     <mergeCell ref="A58:N58"/>
+    <mergeCell ref="A63:N63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10807,7 +10943,7 @@
         </is>
       </c>
       <c r="B1" s="26" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -10817,7 +10953,7 @@
         </is>
       </c>
       <c r="B2" s="26" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -10827,7 +10963,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
@@ -10837,7 +10973,7 @@
         </is>
       </c>
       <c r="B4" s="26" t="n">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
@@ -10847,7 +10983,7 @@
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>423</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6">
@@ -10857,7 +10993,7 @@
         </is>
       </c>
       <c r="B6" s="26" t="n">
-        <v>254</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7">
@@ -10867,7 +11003,7 @@
         </is>
       </c>
       <c r="B7" s="26" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -10877,7 +11013,7 @@
         </is>
       </c>
       <c r="B8" s="26" t="n">
-        <v>78</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9">
@@ -10887,7 +11023,7 @@
         </is>
       </c>
       <c r="B9" s="26" t="n">
-        <v>121</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -10918,17 +11054,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1194 Spools</t>
+          <t>1188 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1045 Workable</t>
+          <t>1081 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>965 Issued</t>
+          <t>1081 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -10981,7 +11117,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11018,7 +11154,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11038,7 +11174,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11090,7 +11226,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>130.9</v>
+        <v>112.3</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -11173,17 +11309,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1194 Spools</t>
+          <t>1188 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1045 Workable</t>
+          <t>1081 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>965 Issued</t>
+          <t>1081 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11236,7 +11372,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11273,7 +11409,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11293,7 +11429,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11345,7 +11481,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>75.7</v>
+        <v>57.1</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -11404,17 +11540,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1194 Spools</t>
+          <t>1188 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1045 Workable</t>
+          <t>1081 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>965 Issued</t>
+          <t>1081 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11467,7 +11603,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11504,7 +11640,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11681,7 +11817,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
@@ -11722,17 +11858,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1194 Spools</t>
+          <t>1188 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1045 Workable</t>
+          <t>1081 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>965 Issued</t>
+          <t>1081 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11793,7 +11929,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11816,7 +11952,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11923,7 +12059,7 @@
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
       <c r="E9" s="22" t="n">
-        <v>965</v>
+        <v>1081</v>
       </c>
       <c r="F9" s="5" t="n"/>
       <c r="G9" s="5" t="n"/>
@@ -11942,7 +12078,7 @@
       <c r="C10" s="5" t="n"/>
       <c r="D10" s="5" t="n"/>
       <c r="E10" s="22" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="F10" s="5" t="n"/>
       <c r="G10" s="5" t="n"/>
@@ -11980,7 +12116,7 @@
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="22" t="n">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F12" s="5" t="n"/>
       <c r="G12" s="5" t="n"/>
@@ -12027,7 +12163,7 @@
         <v/>
       </c>
       <c r="E14" s="24" t="n">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="F14" s="23" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add BOM discrepancies for PMs and Spools
</commit_message>
<xml_diff>
--- a/database/7052/JobSummary.xlsx
+++ b/database/7052/JobSummary.xlsx
@@ -4478,19 +4478,19 @@
       <c r="B1" s="51" t="n"/>
       <c r="C1" s="52" t="inlineStr">
         <is>
-          <t>1188  Spools</t>
+          <t>1295  Spools</t>
         </is>
       </c>
       <c r="D1" s="53" t="n"/>
       <c r="E1" s="54" t="inlineStr">
         <is>
-          <t>1081  Workable</t>
+          <t>931  Workable</t>
         </is>
       </c>
       <c r="F1" s="55" t="n"/>
       <c r="G1" s="52" t="inlineStr">
         <is>
-          <t>1081  Issued</t>
+          <t>1107  Issued</t>
         </is>
       </c>
       <c r="H1" s="56" t="n"/>
@@ -5540,39 +5540,39 @@
         <v>0</v>
       </c>
       <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="G34" s="1" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J34" s="1" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M34" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>51.6%</t>
         </is>
       </c>
       <c r="N34" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>15.0%</t>
         </is>
       </c>
     </row>
@@ -5654,19 +5654,19 @@
         <v>2</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="1" t="n">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
@@ -5675,12 +5675,12 @@
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>62.6%</t>
+          <t>97.6%</t>
         </is>
       </c>
       <c r="N36" s="1" t="inlineStr">
         <is>
-          <t>41.5%</t>
+          <t>87.8%</t>
         </is>
       </c>
     </row>
@@ -5702,39 +5702,39 @@
         <v>0</v>
       </c>
       <c r="E37" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="H37" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="G37" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="H37" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>43</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L37" s="1" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M37" s="1" t="inlineStr">
+        <is>
           <t>97.8%</t>
         </is>
       </c>
-      <c r="M37" s="1" t="inlineStr">
-        <is>
-          <t>95.6%</t>
-        </is>
-      </c>
       <c r="N37" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -5750,45 +5750,45 @@
         </is>
       </c>
       <c r="C38" s="1" t="n">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G38" s="1" t="n">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="J38" s="1" t="n">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>192</v>
+        <v>109</v>
       </c>
       <c r="L38" s="1" t="inlineStr">
         <is>
-          <t>90.2%</t>
+          <t>91.6%</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
         <is>
-          <t>78.4%</t>
+          <t>93.7%</t>
         </is>
       </c>
       <c r="N38" s="1" t="inlineStr">
         <is>
-          <t>24.7%</t>
+          <t>54.0%</t>
         </is>
       </c>
     </row>
@@ -5804,45 +5804,45 @@
         </is>
       </c>
       <c r="C39" s="1" t="n">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="G39" s="1" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J39" s="1" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="L39" s="1" t="inlineStr">
         <is>
-          <t>83.7%</t>
+          <t>49.0%</t>
         </is>
       </c>
       <c r="M39" s="1" t="inlineStr">
         <is>
-          <t>80.2%</t>
+          <t>47.0%</t>
         </is>
       </c>
       <c r="N39" s="1" t="inlineStr">
         <is>
-          <t>25.6%</t>
+          <t>18.5%</t>
         </is>
       </c>
     </row>
@@ -5858,45 +5858,45 @@
         </is>
       </c>
       <c r="C40" s="1" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="J40" s="1" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="L40" s="1" t="inlineStr">
         <is>
-          <t>75.6%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>73.3%</t>
+          <t>44.7%</t>
         </is>
       </c>
       <c r="N40" s="1" t="inlineStr">
         <is>
-          <t>21.1%</t>
+          <t>22.7%</t>
         </is>
       </c>
     </row>
@@ -5924,19 +5924,19 @@
         <v>1</v>
       </c>
       <c r="G41" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J41" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L41" s="1" t="inlineStr">
         <is>
@@ -5945,12 +5945,12 @@
       </c>
       <c r="M41" s="1" t="inlineStr">
         <is>
-          <t>95.2%</t>
+          <t>97.6%</t>
         </is>
       </c>
       <c r="N41" s="1" t="inlineStr">
         <is>
-          <t>19.0%</t>
+          <t>28.6%</t>
         </is>
       </c>
     </row>
@@ -5984,7 +5984,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J42" s="1" t="n">
         <v>0</v>
@@ -6023,7 +6023,7 @@
         <v>158</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>147</v>
@@ -6032,19 +6032,19 @@
         <v>11</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J43" s="1" t="n">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="L43" s="1" t="inlineStr">
         <is>
@@ -6053,12 +6053,12 @@
       </c>
       <c r="M43" s="1" t="inlineStr">
         <is>
-          <t>90.5%</t>
+          <t>92.4%</t>
         </is>
       </c>
       <c r="N43" s="1" t="inlineStr">
         <is>
-          <t>54.4%</t>
+          <t>77.2%</t>
         </is>
       </c>
     </row>
@@ -6092,7 +6092,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J44" s="1" t="n">
         <v>2</v>
@@ -6131,42 +6131,42 @@
         <v>39</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G45" s="1" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H45" s="1" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K45" s="1" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L45" s="1" t="inlineStr">
         <is>
-          <t>61.5%</t>
+          <t>64.1%</t>
         </is>
       </c>
       <c r="M45" s="1" t="inlineStr">
         <is>
-          <t>35.9%</t>
+          <t>48.7%</t>
         </is>
       </c>
       <c r="N45" s="1" t="inlineStr">
         <is>
-          <t>23.1%</t>
+          <t>30.8%</t>
         </is>
       </c>
     </row>
@@ -6200,7 +6200,7 @@
         <v>5</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J46" s="1" t="n">
         <v>0</v>
@@ -6308,13 +6308,13 @@
         <v>0</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J48" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K48" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L48" s="1" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
       </c>
       <c r="N48" s="1" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>55.6%</t>
         </is>
       </c>
     </row>
@@ -6356,20 +6356,20 @@
         <v>0</v>
       </c>
       <c r="G49" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="K49" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="J49" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K49" s="1" t="n">
-        <v>19</v>
-      </c>
       <c r="L49" s="1" t="inlineStr">
         <is>
           <t>100%</t>
@@ -6377,12 +6377,12 @@
       </c>
       <c r="M49" s="1" t="inlineStr">
         <is>
-          <t>95.5%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N49" s="1" t="inlineStr">
         <is>
-          <t>13.6%</t>
+          <t>63.6%</t>
         </is>
       </c>
     </row>
@@ -6416,13 +6416,13 @@
         <v>0</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J50" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K50" s="1" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L50" s="1" t="inlineStr">
         <is>
@@ -6436,7 +6436,7 @@
       </c>
       <c r="N50" s="1" t="inlineStr">
         <is>
-          <t>12.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
     </row>
@@ -6464,19 +6464,19 @@
         <v>6</v>
       </c>
       <c r="G51" s="1" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H51" s="1" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I51" s="1" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J51" s="1" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K51" s="1" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L51" s="1" t="inlineStr">
         <is>
@@ -6485,12 +6485,12 @@
       </c>
       <c r="M51" s="1" t="inlineStr">
         <is>
-          <t>77.4%</t>
+          <t>86.8%</t>
         </is>
       </c>
       <c r="N51" s="1" t="inlineStr">
         <is>
-          <t>15.1%</t>
+          <t>26.4%</t>
         </is>
       </c>
     </row>
@@ -6554,45 +6554,45 @@
       </c>
       <c r="B53" s="76" t="n"/>
       <c r="C53" s="76" t="n">
-        <v>1188</v>
+        <v>1295</v>
       </c>
       <c r="D53" s="76" t="n">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E53" s="76" t="n">
-        <v>1082</v>
+        <v>931</v>
       </c>
       <c r="F53" s="76" t="n">
-        <v>106</v>
+        <v>364</v>
       </c>
       <c r="G53" s="76" t="n">
-        <v>823</v>
+        <v>986</v>
       </c>
       <c r="H53" s="76" t="n">
-        <v>365</v>
+        <v>309</v>
       </c>
       <c r="I53" s="76" t="n">
-        <v>330</v>
+        <v>448</v>
       </c>
       <c r="J53" s="76" t="n">
-        <v>275</v>
+        <v>527</v>
       </c>
       <c r="K53" s="76" t="n">
-        <v>913</v>
+        <v>768</v>
       </c>
       <c r="L53" s="76" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="M53" s="76" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="N53" s="76" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>41%</t>
         </is>
       </c>
     </row>
@@ -6622,7 +6622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6654,6 +6654,180 @@
       <c r="D1" s="27" t="inlineStr">
         <is>
           <t>PM In Status Report (Not in Line List)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>216-1</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-564-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>241-2</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-565-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>296-3</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-568-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>328-2</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-573-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>331-1</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-574-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>388-1</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-575-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>7052-CCW-VALVE-576-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>7052-CS-VALVE-569-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>7052-CS-VALVE-570-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>7052-CW-VALVE-566-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>7052-CW-VALVE-567-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>7052-GN-VALVE-563-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>7052-GN-VALVE-571-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>7052-GN-VALVE-572-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>PM110XA-CS-99999.09-4</t>
         </is>
       </c>
     </row>
@@ -6786,39 +6960,39 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>153</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" s="5" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>51.6%</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>15.0%</t>
         </is>
       </c>
     </row>
@@ -6900,19 +7074,19 @@
         <v>2</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
@@ -6921,12 +7095,12 @@
       </c>
       <c r="M5" s="5" t="inlineStr">
         <is>
-          <t>62.6%</t>
+          <t>97.6%</t>
         </is>
       </c>
       <c r="N5" s="5" t="inlineStr">
         <is>
-          <t>41.5%</t>
+          <t>87.8%</t>
         </is>
       </c>
     </row>
@@ -6948,39 +7122,39 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="H6" s="5" t="n">
         <v>1</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>43</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
           <t>97.8%</t>
         </is>
       </c>
-      <c r="M6" s="5" t="inlineStr">
-        <is>
-          <t>95.6%</t>
-        </is>
-      </c>
       <c r="N6" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -6996,45 +7170,45 @@
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>192</v>
+        <v>109</v>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>90.2%</t>
+          <t>91.6%</t>
         </is>
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>78.4%</t>
+          <t>93.7%</t>
         </is>
       </c>
       <c r="N7" s="5" t="inlineStr">
         <is>
-          <t>24.7%</t>
+          <t>54.0%</t>
         </is>
       </c>
     </row>
@@ -7050,45 +7224,45 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>83.7%</t>
+          <t>49.0%</t>
         </is>
       </c>
       <c r="M8" s="5" t="inlineStr">
         <is>
-          <t>80.2%</t>
+          <t>47.0%</t>
         </is>
       </c>
       <c r="N8" s="5" t="inlineStr">
         <is>
-          <t>25.6%</t>
+          <t>18.5%</t>
         </is>
       </c>
     </row>
@@ -7104,45 +7278,45 @@
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>75.6%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="M9" s="5" t="inlineStr">
         <is>
-          <t>73.3%</t>
+          <t>44.7%</t>
         </is>
       </c>
       <c r="N9" s="5" t="inlineStr">
         <is>
-          <t>21.1%</t>
+          <t>22.7%</t>
         </is>
       </c>
     </row>
@@ -7170,19 +7344,19 @@
         <v>1</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
@@ -7191,12 +7365,12 @@
       </c>
       <c r="M10" s="5" t="inlineStr">
         <is>
-          <t>95.2%</t>
+          <t>97.6%</t>
         </is>
       </c>
       <c r="N10" s="5" t="inlineStr">
         <is>
-          <t>19.0%</t>
+          <t>28.6%</t>
         </is>
       </c>
     </row>
@@ -7230,7 +7404,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J11" s="5" t="n">
         <v>0</v>
@@ -7269,7 +7443,7 @@
         <v>158</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>147</v>
@@ -7278,19 +7452,19 @@
         <v>11</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
@@ -7299,12 +7473,12 @@
       </c>
       <c r="M12" s="5" t="inlineStr">
         <is>
-          <t>90.5%</t>
+          <t>92.4%</t>
         </is>
       </c>
       <c r="N12" s="5" t="inlineStr">
         <is>
-          <t>54.4%</t>
+          <t>77.2%</t>
         </is>
       </c>
     </row>
@@ -7338,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>2</v>
@@ -7377,42 +7551,42 @@
         <v>39</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>61.5%</t>
+          <t>64.1%</t>
         </is>
       </c>
       <c r="M14" s="5" t="inlineStr">
         <is>
-          <t>35.9%</t>
+          <t>48.7%</t>
         </is>
       </c>
       <c r="N14" s="5" t="inlineStr">
         <is>
-          <t>23.1%</t>
+          <t>30.8%</t>
         </is>
       </c>
     </row>
@@ -7446,7 +7620,7 @@
         <v>5</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
@@ -7554,13 +7728,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
@@ -7574,7 +7748,7 @@
       </c>
       <c r="N17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>55.6%</t>
         </is>
       </c>
     </row>
@@ -7602,20 +7776,20 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K18" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="J18" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="K18" s="5" t="n">
-        <v>19</v>
-      </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
           <t>100%</t>
@@ -7623,12 +7797,12 @@
       </c>
       <c r="M18" s="5" t="inlineStr">
         <is>
-          <t>95.5%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N18" s="5" t="inlineStr">
         <is>
-          <t>13.6%</t>
+          <t>63.6%</t>
         </is>
       </c>
     </row>
@@ -7662,13 +7836,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L19" s="5" t="inlineStr">
         <is>
@@ -7682,7 +7856,7 @@
       </c>
       <c r="N19" s="5" t="inlineStr">
         <is>
-          <t>12.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
     </row>
@@ -7710,19 +7884,19 @@
         <v>6</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L20" s="5" t="inlineStr">
         <is>
@@ -7731,12 +7905,12 @@
       </c>
       <c r="M20" s="5" t="inlineStr">
         <is>
-          <t>77.4%</t>
+          <t>86.8%</t>
         </is>
       </c>
       <c r="N20" s="5" t="inlineStr">
         <is>
-          <t>15.1%</t>
+          <t>26.4%</t>
         </is>
       </c>
     </row>
@@ -7800,45 +7974,45 @@
       </c>
       <c r="B22" s="79" t="n"/>
       <c r="C22" s="79" t="n">
-        <v>1188</v>
+        <v>1295</v>
       </c>
       <c r="D22" s="79" t="n">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E22" s="79" t="n">
-        <v>1081</v>
+        <v>931</v>
       </c>
       <c r="F22" s="79" t="n">
-        <v>107</v>
+        <v>364</v>
       </c>
       <c r="G22" s="79" t="n">
-        <v>823</v>
+        <v>986</v>
       </c>
       <c r="H22" s="79" t="n">
-        <v>365</v>
+        <v>309</v>
       </c>
       <c r="I22" s="79" t="n">
-        <v>330</v>
+        <v>448</v>
       </c>
       <c r="J22" s="79" t="n">
-        <v>275</v>
+        <v>527</v>
       </c>
       <c r="K22" s="79" t="n">
-        <v>913</v>
+        <v>768</v>
       </c>
       <c r="L22" s="79" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="M22" s="79" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="N22" s="79" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>41%</t>
         </is>
       </c>
     </row>
@@ -7974,7 +8148,7 @@
         <v>154</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>143</v>
@@ -7989,13 +8163,13 @@
         <v>12</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
@@ -8009,7 +8183,7 @@
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
-          <t>55.8%</t>
+          <t>79.2%</t>
         </is>
       </c>
     </row>
@@ -8043,7 +8217,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J4" s="5" t="n">
         <v>2</v>
@@ -8100,10 +8274,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
@@ -8117,7 +8291,7 @@
       </c>
       <c r="N5" s="5" t="inlineStr">
         <is>
-          <t>23.1%</t>
+          <t>92.3%</t>
         </is>
       </c>
     </row>
@@ -8145,19 +8319,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
@@ -8166,12 +8340,12 @@
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>91.7%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N6" s="5" t="inlineStr">
         <is>
-          <t>16.7%</t>
+          <t>75.0%</t>
         </is>
       </c>
     </row>
@@ -8199,19 +8373,19 @@
         <v>0</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
@@ -8220,12 +8394,12 @@
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>86.8%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N7" s="5" t="inlineStr">
         <is>
-          <t>71.1%</t>
+          <t>94.7%</t>
         </is>
       </c>
     </row>
@@ -8243,10 +8417,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="n">
         <v>31</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0</v>
@@ -8265,7 +8439,7 @@
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M8" s="5" t="inlineStr">
@@ -8290,42 +8464,42 @@
         <v>290</v>
       </c>
       <c r="D9" s="79" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E9" s="79" t="n">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="F9" s="79" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="G9" s="79" t="n">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="H9" s="79" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I9" s="79" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="J9" s="79" t="n">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="K9" s="79" t="n">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="L9" s="79" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="M9" s="79" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="N9" s="79" t="inlineStr">
         <is>
-          <t>41%</t>
+          <t>62%</t>
         </is>
       </c>
     </row>
@@ -8454,13 +8628,13 @@
         <v>0</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L13" s="5" t="inlineStr">
         <is>
@@ -8474,7 +8648,7 @@
       </c>
       <c r="N13" s="5" t="inlineStr">
         <is>
-          <t>10.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -8508,13 +8682,13 @@
         <v>0</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
@@ -8528,7 +8702,7 @@
       </c>
       <c r="N14" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>25.0%</t>
         </is>
       </c>
     </row>
@@ -8562,13 +8736,13 @@
         <v>0</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L15" s="5" t="inlineStr">
         <is>
@@ -8582,7 +8756,7 @@
       </c>
       <c r="N15" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>17.9%</t>
         </is>
       </c>
     </row>
@@ -8670,13 +8844,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L17" s="5" t="inlineStr">
         <is>
@@ -8690,7 +8864,7 @@
       </c>
       <c r="N17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>55.6%</t>
         </is>
       </c>
     </row>
@@ -8712,39 +8886,39 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="H18" s="5" t="n">
         <v>1</v>
-      </c>
-      <c r="G18" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="H18" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="I18" s="5" t="n">
         <v>43</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L18" s="5" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="M18" s="5" t="inlineStr">
+        <is>
           <t>97.8%</t>
         </is>
       </c>
-      <c r="M18" s="5" t="inlineStr">
-        <is>
-          <t>95.6%</t>
-        </is>
-      </c>
       <c r="N18" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -8812,45 +8986,45 @@
         </is>
       </c>
       <c r="C20" s="5" t="n">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="L20" s="5" t="inlineStr">
         <is>
-          <t>88.5%</t>
+          <t>89.9%</t>
         </is>
       </c>
       <c r="M20" s="5" t="inlineStr">
         <is>
-          <t>77.0%</t>
+          <t>92.5%</t>
         </is>
       </c>
       <c r="N20" s="5" t="inlineStr">
         <is>
-          <t>16.6%</t>
+          <t>46.2%</t>
         </is>
       </c>
     </row>
@@ -8866,45 +9040,45 @@
         </is>
       </c>
       <c r="C21" s="5" t="n">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="J21" s="5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="L21" s="5" t="inlineStr">
         <is>
-          <t>68.9%</t>
+          <t>44.6%</t>
         </is>
       </c>
       <c r="M21" s="5" t="inlineStr">
         <is>
-          <t>65.6%</t>
+          <t>33.9%</t>
         </is>
       </c>
       <c r="N21" s="5" t="inlineStr">
         <is>
-          <t>3.3%</t>
+          <t>6.6%</t>
         </is>
       </c>
     </row>
@@ -8920,45 +9094,45 @@
         </is>
       </c>
       <c r="C22" s="5" t="n">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="L22" s="5" t="inlineStr">
         <is>
-          <t>80.7%</t>
+          <t>41.8%</t>
         </is>
       </c>
       <c r="M22" s="5" t="inlineStr">
         <is>
-          <t>75.4%</t>
+          <t>36.9%</t>
         </is>
       </c>
       <c r="N22" s="5" t="inlineStr">
         <is>
-          <t>1.8%</t>
+          <t>4.9%</t>
         </is>
       </c>
     </row>
@@ -8995,10 +9169,10 @@
         <v>20</v>
       </c>
       <c r="J23" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L23" s="5" t="inlineStr">
         <is>
@@ -9012,7 +9186,7 @@
       </c>
       <c r="N23" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>
@@ -9046,7 +9220,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="J24" s="5" t="n">
         <v>0</v>
@@ -9094,10 +9268,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H25" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I25" s="5" t="n">
         <v>0</v>
@@ -9115,7 +9289,7 @@
       </c>
       <c r="M25" s="5" t="inlineStr">
         <is>
-          <t>25.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N25" s="5" t="inlineStr">
@@ -9154,7 +9328,7 @@
         <v>5</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J26" s="5" t="n">
         <v>0</v>
@@ -9240,45 +9414,45 @@
       </c>
       <c r="B28" s="79" t="n"/>
       <c r="C28" s="79" t="n">
-        <v>494</v>
+        <v>601</v>
       </c>
       <c r="D28" s="79" t="n">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="E28" s="79" t="n">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="F28" s="79" t="n">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="G28" s="79" t="n">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="H28" s="79" t="n">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="I28" s="79" t="n">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="J28" s="79" t="n">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="K28" s="79" t="n">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="L28" s="79" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="M28" s="79" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="N28" s="79" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>22%</t>
         </is>
       </c>
     </row>
@@ -9407,7 +9581,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>0</v>
@@ -9461,7 +9635,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J33" s="5" t="n">
         <v>0</v>
@@ -9515,7 +9689,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J34" s="5" t="n">
         <v>0</v>
@@ -9565,7 +9739,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="79" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J35" s="79" t="n">
         <v>0</v>
@@ -9708,19 +9882,19 @@
         <v>2</v>
       </c>
       <c r="G39" s="5" t="n">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="I39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J39" s="5" t="n">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="L39" s="5" t="inlineStr">
         <is>
@@ -9729,12 +9903,12 @@
       </c>
       <c r="M39" s="5" t="inlineStr">
         <is>
-          <t>63.1%</t>
+          <t>97.5%</t>
         </is>
       </c>
       <c r="N39" s="5" t="inlineStr">
         <is>
-          <t>41.8%</t>
+          <t>87.7%</t>
         </is>
       </c>
     </row>
@@ -9762,10 +9936,10 @@
         <v>6</v>
       </c>
       <c r="G40" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H40" s="5" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I40" s="5" t="n">
         <v>0</v>
@@ -9783,7 +9957,7 @@
       </c>
       <c r="M40" s="5" t="inlineStr">
         <is>
-          <t>35.3%</t>
+          <t>58.8%</t>
         </is>
       </c>
       <c r="N40" s="5" t="inlineStr">
@@ -9861,42 +10035,42 @@
         <v>35</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="H42" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I42" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="H42" s="5" t="n">
+      <c r="K42" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="I42" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="K42" s="5" t="n">
-        <v>26</v>
-      </c>
       <c r="L42" s="5" t="inlineStr">
         <is>
-          <t>62.9%</t>
+          <t>65.7%</t>
         </is>
       </c>
       <c r="M42" s="5" t="inlineStr">
         <is>
+          <t>48.6%</t>
+        </is>
+      </c>
+      <c r="N42" s="5" t="inlineStr">
+        <is>
           <t>34.3%</t>
-        </is>
-      </c>
-      <c r="N42" s="5" t="inlineStr">
-        <is>
-          <t>25.7%</t>
         </is>
       </c>
     </row>
@@ -9914,39 +10088,39 @@
         <v>0</v>
       </c>
       <c r="E43" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5" t="n">
         <v>122</v>
       </c>
-      <c r="F43" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="G43" s="5" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>122</v>
+        <v>43</v>
       </c>
       <c r="I43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="5" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K43" s="5" t="n">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="L43" s="5" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="M43" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>64.8%</t>
         </is>
       </c>
       <c r="N43" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>18.9%</t>
         </is>
       </c>
     </row>
@@ -9961,42 +10135,42 @@
         <v>299</v>
       </c>
       <c r="D44" s="79" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E44" s="79" t="n">
-        <v>278</v>
+        <v>157</v>
       </c>
       <c r="F44" s="79" t="n">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="G44" s="79" t="n">
-        <v>96</v>
+        <v>226</v>
       </c>
       <c r="H44" s="79" t="n">
-        <v>203</v>
+        <v>73</v>
       </c>
       <c r="I44" s="79" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="79" t="n">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="K44" s="79" t="n">
-        <v>232</v>
+        <v>150</v>
       </c>
       <c r="L44" s="79" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>53%</t>
         </is>
       </c>
       <c r="M44" s="79" t="inlineStr">
         <is>
-          <t>32%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="N44" s="79" t="inlineStr">
         <is>
-          <t>22%</t>
+          <t>50%</t>
         </is>
       </c>
     </row>
@@ -10119,20 +10293,20 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H48" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H48" s="5" t="n">
+      <c r="K48" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I48" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="K48" s="5" t="n">
-        <v>2</v>
-      </c>
       <c r="L48" s="5" t="inlineStr">
         <is>
           <t>100%</t>
@@ -10140,12 +10314,12 @@
       </c>
       <c r="M48" s="5" t="inlineStr">
         <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="N48" s="5" t="inlineStr">
+        <is>
           <t>75.0%</t>
-        </is>
-      </c>
-      <c r="N48" s="5" t="inlineStr">
-        <is>
-          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -10173,19 +10347,19 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K49" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L49" s="5" t="inlineStr">
         <is>
@@ -10194,12 +10368,12 @@
       </c>
       <c r="M49" s="5" t="inlineStr">
         <is>
-          <t>90.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N49" s="5" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>100%</t>
         </is>
       </c>
     </row>
@@ -10223,19 +10397,19 @@
         <v>0</v>
       </c>
       <c r="G50" s="79" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H50" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I50" s="79" t="n">
         <v>0</v>
       </c>
       <c r="J50" s="79" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K50" s="79" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L50" s="79" t="inlineStr">
         <is>
@@ -10244,12 +10418,12 @@
       </c>
       <c r="M50" s="79" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N50" s="79" t="inlineStr">
         <is>
-          <t>71%</t>
+          <t>93%</t>
         </is>
       </c>
     </row>
@@ -10366,10 +10540,10 @@
         <v>0</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F54" s="5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G54" s="5" t="n">
         <v>26</v>
@@ -10381,24 +10555,24 @@
         <v>21</v>
       </c>
       <c r="J54" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K54" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L54" s="5" t="inlineStr">
         <is>
+          <t>79.3%</t>
+        </is>
+      </c>
+      <c r="M54" s="5" t="inlineStr">
+        <is>
           <t>89.7%</t>
         </is>
       </c>
-      <c r="M54" s="5" t="inlineStr">
-        <is>
-          <t>89.7%</t>
-        </is>
-      </c>
       <c r="N54" s="5" t="inlineStr">
         <is>
-          <t>72.4%</t>
+          <t>75.9%</t>
         </is>
       </c>
     </row>
@@ -10435,10 +10609,10 @@
         <v>17</v>
       </c>
       <c r="J55" s="5" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K55" s="5" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L55" s="5" t="inlineStr">
         <is>
@@ -10452,7 +10626,7 @@
       </c>
       <c r="N55" s="5" t="inlineStr">
         <is>
-          <t>58.6%</t>
+          <t>89.7%</t>
         </is>
       </c>
     </row>
@@ -10470,10 +10644,10 @@
         <v>0</v>
       </c>
       <c r="E56" s="79" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F56" s="79" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G56" s="79" t="n">
         <v>52</v>
@@ -10485,24 +10659,24 @@
         <v>38</v>
       </c>
       <c r="J56" s="79" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="K56" s="79" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L56" s="79" t="inlineStr">
         <is>
+          <t>84%</t>
+        </is>
+      </c>
+      <c r="M56" s="79" t="inlineStr">
+        <is>
           <t>90%</t>
         </is>
       </c>
-      <c r="M56" s="79" t="inlineStr">
-        <is>
-          <t>90%</t>
-        </is>
-      </c>
       <c r="N56" s="79" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>83%</t>
         </is>
       </c>
     </row>
@@ -10625,19 +10799,19 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I60" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="K60" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" s="5" t="inlineStr">
         <is>
@@ -10646,12 +10820,12 @@
       </c>
       <c r="M60" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N60" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100%</t>
         </is>
       </c>
     </row>
@@ -10675,19 +10849,19 @@
         <v>0</v>
       </c>
       <c r="G61" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="I61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="79" t="n">
-        <v>0</v>
-      </c>
       <c r="K61" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" s="79" t="inlineStr">
         <is>
@@ -10696,12 +10870,12 @@
       </c>
       <c r="M61" s="79" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N61" s="79" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100%</t>
         </is>
       </c>
     </row>
@@ -10943,7 +11117,7 @@
         </is>
       </c>
       <c r="B1" s="26" t="n">
-        <v>26</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
@@ -10953,7 +11127,7 @@
         </is>
       </c>
       <c r="B2" s="26" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -10963,7 +11137,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>143</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -10973,7 +11147,7 @@
         </is>
       </c>
       <c r="B4" s="26" t="n">
-        <v>115</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -10983,7 +11157,7 @@
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>198</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
@@ -10993,7 +11167,7 @@
         </is>
       </c>
       <c r="B6" s="26" t="n">
-        <v>274</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7">
@@ -11003,7 +11177,7 @@
         </is>
       </c>
       <c r="B7" s="26" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -11013,7 +11187,7 @@
         </is>
       </c>
       <c r="B8" s="26" t="n">
-        <v>275</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9">
@@ -11023,7 +11197,7 @@
         </is>
       </c>
       <c r="B9" s="26" t="n">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -11054,17 +11228,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1188 Spools</t>
+          <t>1295 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1081 Workable</t>
+          <t>931 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>1081 Issued</t>
+          <t>1107 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11134,7 +11308,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11154,7 +11328,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11174,7 +11348,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11226,7 +11400,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>112.3</v>
+        <v>117.7</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -11309,17 +11483,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1188 Spools</t>
+          <t>1295 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1081 Workable</t>
+          <t>931 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>1081 Issued</t>
+          <t>1107 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11372,7 +11546,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11389,7 +11563,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11409,7 +11583,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11481,7 +11655,7 @@
         </is>
       </c>
       <c r="B10" s="11" t="n">
-        <v>57.1</v>
+        <v>98.7</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0</v>
@@ -11540,17 +11714,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1188 Spools</t>
+          <t>1295 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1081 Workable</t>
+          <t>931 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>1081 Issued</t>
+          <t>1107 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11603,7 +11777,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
@@ -11620,7 +11794,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11640,7 +11814,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -11660,7 +11834,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -11712,7 +11886,7 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>55.2</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0</v>
@@ -11817,7 +11991,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
@@ -11858,17 +12032,17 @@
     <row r="1" ht="36" customHeight="1">
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>1188 Spools</t>
+          <t>1295 Spools</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>1081 Workable</t>
+          <t>931 Workable</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>1081 Issued</t>
+          <t>1107 Issued</t>
         </is>
       </c>
       <c r="E1" s="3" t="n"/>
@@ -11952,7 +12126,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0</v>
@@ -11978,7 +12152,7 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
@@ -12004,7 +12178,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
@@ -12030,7 +12204,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>0</v>
@@ -12059,7 +12233,7 @@
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
       <c r="E9" s="22" t="n">
-        <v>1081</v>
+        <v>1107</v>
       </c>
       <c r="F9" s="5" t="n"/>
       <c r="G9" s="5" t="n"/>
@@ -12078,7 +12252,7 @@
       <c r="C10" s="5" t="n"/>
       <c r="D10" s="5" t="n"/>
       <c r="E10" s="22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" s="5" t="n"/>
       <c r="G10" s="5" t="n"/>
@@ -12097,7 +12271,7 @@
       <c r="C11" s="5" t="n"/>
       <c r="D11" s="5" t="n"/>
       <c r="E11" s="22" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F11" s="5" t="n"/>
       <c r="G11" s="5" t="n"/>
@@ -12116,7 +12290,7 @@
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="22" t="n">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="F12" s="5" t="n"/>
       <c r="G12" s="5" t="n"/>
@@ -12135,7 +12309,7 @@
       <c r="C13" s="30" t="n"/>
       <c r="D13" s="30" t="n"/>
       <c r="E13" s="28" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F13" s="5" t="n"/>
       <c r="G13" s="5" t="n"/>
@@ -12163,7 +12337,7 @@
         <v/>
       </c>
       <c r="E14" s="24" t="n">
-        <v>1188</v>
+        <v>1295</v>
       </c>
       <c r="F14" s="23" t="inlineStr">
         <is>

</xml_diff>